<commit_message>
Add optimal design values for lift+cruise
</commit_message>
<xml_diff>
--- a/sheets/estimate_mtow.xlsx
+++ b/sheets/estimate_mtow.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D712EEA-0D35-164F-9722-96E0209E3159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE184964-3C7B-1047-B4B4-56EAE7A28A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15080" windowHeight="18900" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
   </bookViews>
   <sheets>
     <sheet name="multirotor" sheetId="3" r:id="rId1"/>
     <sheet name="lift+cruise" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="141">
   <si>
     <t>!!! Press F9 to recalculate !!!</t>
   </si>
@@ -391,6 +392,75 @@
   </si>
   <si>
     <t>Bisection method for solving W_total_takeoff</t>
+  </si>
+  <si>
+    <t>torque</t>
+  </si>
+  <si>
+    <t>Nm</t>
+  </si>
+  <si>
+    <t>thrust</t>
+  </si>
+  <si>
+    <t>n_rotor</t>
+  </si>
+  <si>
+    <t>P_motor</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>W_rotor+hubs</t>
+  </si>
+  <si>
+    <t>W_motor</t>
+  </si>
+  <si>
+    <t>W_motor_controller</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>technology_factor</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>helicopter</t>
+  </si>
+  <si>
+    <t>tiltrotor</t>
+  </si>
+  <si>
+    <t>tiltwing</t>
+  </si>
+  <si>
+    <t>Gross weight</t>
+  </si>
+  <si>
+    <t>ft2</t>
+  </si>
+  <si>
+    <t>Eqv flat plat area (f)</t>
+  </si>
+  <si>
+    <t>K_eqv</t>
+  </si>
+  <si>
+    <t>Eqv_flat_plat_calc</t>
+  </si>
+  <si>
+    <t>L/D</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>AR</t>
   </si>
 </sst>
 </file>
@@ -506,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -538,20 +608,18 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1592,19 +1660,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22.74</c:v>
+                  <c:v>33.369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.69</c:v>
+                  <c:v>17.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.12</c:v>
+                  <c:v>11.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.51</c:v>
+                  <c:v>32.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.94</c:v>
+                  <c:v>5.86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3221,8 +3289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22671EB-89B6-F54E-A7EC-520F7563A407}">
   <dimension ref="B1:AJ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3253,11 +3321,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="2:36" x14ac:dyDescent="0.2">
       <c r="P2" s="6" t="s">
@@ -3271,18 +3339,18 @@
       <c r="B3" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
       <c r="F3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="J3" s="19" t="s">
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="J3" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
       <c r="P3" s="7" t="s">
         <v>76</v>
       </c>
@@ -3503,7 +3571,7 @@
         <v>500</v>
       </c>
       <c r="AC5" s="8">
-        <f t="dataTable" ref="AC5:AC44" dt2D="0" dtr="0" r1="C15" ca="1"/>
+        <f t="dataTable" ref="AC5:AC44" dt2D="0" dtr="0" r1="C15"/>
         <v>-264.34947063042887</v>
       </c>
       <c r="AD5" s="9">
@@ -3518,7 +3586,7 @@
         <v>1500</v>
       </c>
       <c r="AG5" s="8">
-        <f t="dataTable" ref="AG5:AG44" dt2D="0" dtr="0" r1="C15"/>
+        <f t="dataTable" ref="AG5:AG44" dt2D="0" dtr="0" r1="C15" ca="1"/>
         <v>48.370255085541658</v>
       </c>
       <c r="AH5" s="8">
@@ -3634,8 +3702,8 @@
       <c r="F7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
       <c r="J7" t="s">
         <v>69</v>
       </c>
@@ -3823,8 +3891,8 @@
       <c r="B9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="F9" s="4" t="s">
         <v>40</v>
       </c>
@@ -4007,13 +4075,13 @@
       <c r="F11" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
       <c r="J11" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
       <c r="P11" s="8">
         <v>7</v>
       </c>
@@ -4288,11 +4356,11 @@
       </c>
     </row>
     <row r="14" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="P14" s="8">
         <v>10</v>
       </c>
@@ -4471,11 +4539,11 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
       <c r="P16" s="8">
         <v>12</v>
       </c>
@@ -4859,11 +4927,11 @@
       </c>
     </row>
     <row r="20" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="F20" s="14" t="s">
         <v>97</v>
       </c>
@@ -5366,11 +5434,11 @@
       </c>
     </row>
     <row r="25" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
       <c r="F25" s="15" t="s">
         <v>104</v>
       </c>
@@ -5744,11 +5812,11 @@
       </c>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
       <c r="P29" s="8">
         <v>25</v>
       </c>
@@ -6680,12 +6748,12 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B25:D25"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F11:H11"/>
   </mergeCells>
   <conditionalFormatting sqref="G27">
     <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="FALSE">
@@ -6716,8 +6784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C46306-B19A-E840-A2A2-9C88BDE95F01}">
   <dimension ref="B1:AJ57"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6748,11 +6816,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="2:36" x14ac:dyDescent="0.2">
       <c r="P2" s="6" t="s">
@@ -6766,18 +6834,18 @@
       <c r="B3" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
       <c r="F3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="J3" s="19" t="s">
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="J3" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
       <c r="P3" s="7" t="s">
         <v>76</v>
       </c>
@@ -6851,7 +6919,7 @@
       </c>
       <c r="G4">
         <f xml:space="preserve"> 1/$C$9 * SQRT( ($C$20*$C$34)^3 / (2 * $C$33 * PI() * $C$21^2* $C$5) )</f>
-        <v>370704.43153783563</v>
+        <v>166764.64204991527</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -6861,7 +6929,7 @@
       </c>
       <c r="K4">
         <f xml:space="preserve"> $C$20 * $C$34</f>
-        <v>17258.482001234643</v>
+        <v>11757.8180294921</v>
       </c>
       <c r="L4" t="s">
         <v>37</v>
@@ -6874,14 +6942,14 @@
       </c>
       <c r="R4" s="8">
         <f t="shared" ref="R4:R34" si="0" xml:space="preserve"> $K$20 * TAN($K$17) + $K$21 / (2 * SQRT($K$20^2 + Q4^2)) - Q4</f>
-        <v>0.6534009566313479</v>
+        <v>0.63509455714344953</v>
       </c>
       <c r="S4" s="9">
         <v>1</v>
       </c>
       <c r="T4" s="8">
         <f t="shared" ref="T4:T34" si="1" xml:space="preserve"> $K$20 * TAN($K$17) + $K$21 / (2 * SQRT($K$20^2 + S4^2)) - S4</f>
-        <v>-0.67357508815696088</v>
+        <v>-0.57973927437983719</v>
       </c>
       <c r="U4" s="8">
         <f xml:space="preserve"> (Q4 + S4)/2</f>
@@ -6889,15 +6957,15 @@
       </c>
       <c r="V4" s="8">
         <f t="shared" ref="V4:V34" si="2" xml:space="preserve"> $K$20 * TAN($K$17) + $K$21 / (2 * SQRT($K$20^2 + U4^2)) - U4</f>
-        <v>-0.16427027744759859</v>
+        <v>-7.1737967926194857E-2</v>
       </c>
       <c r="W4" s="8">
         <f>R4*V4</f>
-        <v>-0.10733435643035785</v>
+        <v>-4.5560392970457712E-2</v>
       </c>
       <c r="X4" s="8">
         <f>T4*V4</f>
-        <v>0.11064836661333464</v>
+        <v>4.1589317471016241E-2</v>
       </c>
       <c r="Y4" s="8">
         <f>S4-Q4</f>
@@ -6909,17 +6977,17 @@
       <c r="AB4" s="8"/>
       <c r="AC4" s="8">
         <f>G29</f>
-        <v>1.546140993013978E-10</v>
+        <v>-1.0618350643198937E-10</v>
       </c>
       <c r="AD4" s="8"/>
       <c r="AE4" s="8">
         <f>G29</f>
-        <v>1.546140993013978E-10</v>
+        <v>-1.0618350643198937E-10</v>
       </c>
       <c r="AF4" s="8"/>
       <c r="AG4" s="8">
         <f>G29</f>
-        <v>1.546140993013978E-10</v>
+        <v>-1.0618350643198937E-10</v>
       </c>
       <c r="AH4" s="8"/>
       <c r="AI4" s="8"/>
@@ -6937,7 +7005,7 @@
       </c>
       <c r="G5">
         <f xml:space="preserve"> $C$20 * $C$34 / $C$5</f>
-        <v>2876.4136668724404</v>
+        <v>1959.6363382486834</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
@@ -6947,7 +7015,7 @@
       </c>
       <c r="K5">
         <f xml:space="preserve"> 0.5 * $C$33 * $C$23^2</f>
-        <v>1852.8125000000002</v>
+        <v>1852.8124999999461</v>
       </c>
       <c r="L5" t="s">
         <v>48</v>
@@ -6961,7 +7029,7 @@
       </c>
       <c r="R5" s="8">
         <f t="shared" si="0"/>
-        <v>0.6534009566313479</v>
+        <v>0.63509455714344953</v>
       </c>
       <c r="S5" s="8">
         <f>IF(X4&gt;0, U4, S4)</f>
@@ -6969,7 +7037,7 @@
       </c>
       <c r="T5" s="8">
         <f t="shared" si="1"/>
-        <v>-0.16427027744759859</v>
+        <v>-7.1737967926194857E-2</v>
       </c>
       <c r="U5" s="8">
         <f t="shared" ref="U5:U34" si="3" xml:space="preserve"> (Q5 + S5)/2</f>
@@ -6977,15 +7045,15 @@
       </c>
       <c r="V5" s="8">
         <f t="shared" si="2"/>
-        <v>0.10419045512088293</v>
+        <v>0.19404975122575574</v>
       </c>
       <c r="W5" s="8">
         <f t="shared" ref="W5:W34" si="4">R5*V5</f>
-        <v>6.807814304784042E-2</v>
+        <v>0.1232399408185179</v>
       </c>
       <c r="X5" s="8">
         <f t="shared" ref="X5:X34" si="5">T5*V5</f>
-        <v>-1.7115394970099007E-2</v>
+        <v>-1.3920734829519357E-2</v>
       </c>
       <c r="Y5" s="8">
         <f t="shared" ref="Y5:Y34" si="6">S5-Q5</f>
@@ -6998,31 +7066,31 @@
         <v>500</v>
       </c>
       <c r="AC5" s="8">
-        <f t="dataTable" ref="AC5:AC44" dt2D="0" dtr="0" r1="C20" ca="1"/>
-        <v>-387.71074190676364</v>
+        <f t="dataTable" ref="AC5:AC44" dt2D="0" dtr="0" r1="C20"/>
+        <v>-357.0306442450181</v>
       </c>
       <c r="AD5" s="9">
         <v>2500</v>
       </c>
       <c r="AE5" s="8">
         <f t="dataTable" ref="AE5:AE44" dt2D="0" dtr="0" r1="C20" ca="1"/>
-        <v>17.800327323294368</v>
+        <v>536.38035314613489</v>
       </c>
       <c r="AF5" s="8">
         <f>(AB5+AD5)/2</f>
         <v>1500</v>
       </c>
       <c r="AG5" s="8">
-        <f t="dataTable" ref="AG5:AG44" dt2D="0" dtr="0" r1="C20"/>
-        <v>-47.313913459105152</v>
+        <f t="dataTable" ref="AG5:AG44" dt2D="0" dtr="0" r1="C20" ca="1"/>
+        <v>142.55710353272457</v>
       </c>
       <c r="AH5" s="8">
         <f>AC5*AG5</f>
-        <v>18344.112489742067</v>
+        <v>-50897.254515992398</v>
       </c>
       <c r="AI5" s="8">
         <f>AE5*AG5</f>
-        <v>-842.20314651809463</v>
+        <v>76464.829536372912</v>
       </c>
       <c r="AJ5" s="8">
         <f>AD5-AB5</f>
@@ -7041,7 +7109,7 @@
       </c>
       <c r="K6">
         <f xml:space="preserve"> 1.6 * ($C$20*2.20462/1000)^(2/3) * 0.3048^2</f>
-        <v>0.36693977839770386</v>
+        <v>0.28410413500282999</v>
       </c>
       <c r="L6" t="s">
         <v>21</v>
@@ -7055,7 +7123,7 @@
       </c>
       <c r="R6" s="8">
         <f t="shared" si="0"/>
-        <v>0.10419045512088293</v>
+        <v>0.19404975122575574</v>
       </c>
       <c r="S6" s="8">
         <f t="shared" ref="S6:S34" si="8">IF(X5&gt;0, U5, S5)</f>
@@ -7063,7 +7131,7 @@
       </c>
       <c r="T6" s="8">
         <f t="shared" si="1"/>
-        <v>-0.16427027744759859</v>
+        <v>-7.1737967926194857E-2</v>
       </c>
       <c r="U6" s="8">
         <f t="shared" si="3"/>
@@ -7071,15 +7139,15 @@
       </c>
       <c r="V6" s="8">
         <f t="shared" si="2"/>
-        <v>-3.3089506961332005E-2</v>
+        <v>5.8563738317039926E-2</v>
       </c>
       <c r="W6" s="8">
         <f t="shared" si="4"/>
-        <v>-3.4476107900268055E-3</v>
+        <v>1.1364278851271857E-2</v>
       </c>
       <c r="X6" s="8">
         <f t="shared" si="5"/>
-        <v>5.4356224891422529E-3</v>
+        <v>-4.2012435810258788E-3</v>
       </c>
       <c r="Y6" s="8">
         <f t="shared" si="6"/>
@@ -7090,32 +7158,32 @@
       </c>
       <c r="AB6" s="8">
         <f>IF(AH5&gt;0,AF5,AB5)</f>
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="AC6" s="8">
-        <v>-47.313913459105152</v>
+        <v>-357.0306442450181</v>
       </c>
       <c r="AD6" s="8">
         <f>IF(AI5&gt;0,AF5,AD5)</f>
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="AE6" s="8">
-        <v>17.800327323294368</v>
+        <v>142.55710353272457</v>
       </c>
       <c r="AF6" s="8">
         <f t="shared" ref="AF6:AF44" si="9">(AB6+AD6)/2</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="AG6" s="8">
-        <v>25.674914961811965</v>
+        <v>-98.697740238587812</v>
       </c>
       <c r="AH6" s="8">
         <f t="shared" ref="AH6:AH44" si="10">AC6*AG6</f>
-        <v>-1214.7807045730553</v>
+        <v>35238.117782910449</v>
       </c>
       <c r="AI6" s="8">
         <f t="shared" ref="AI6:AI44" si="11">AE6*AG6</f>
-        <v>457.02189031800089</v>
+        <v>-14070.063973638318</v>
       </c>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ44" si="12">AD6-AB6</f>
@@ -7132,49 +7200,49 @@
       <c r="F7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
       <c r="J7" t="s">
         <v>68</v>
       </c>
       <c r="K7">
         <f xml:space="preserve"> K6 / $C$24</f>
-        <v>5.7334340374641225E-2</v>
+        <v>2.6861702975669303E-2</v>
       </c>
       <c r="P7" s="8">
         <v>3</v>
       </c>
       <c r="Q7" s="8">
         <f t="shared" si="7"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="R7" s="8">
         <f t="shared" si="0"/>
-        <v>0.10419045512088293</v>
+        <v>5.8563738317039926E-2</v>
       </c>
       <c r="S7" s="8">
         <f t="shared" si="8"/>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="T7" s="8">
         <f t="shared" si="1"/>
-        <v>-3.3089506961332005E-2</v>
+        <v>-7.1737967926194857E-2</v>
       </c>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>0.3125</v>
+        <v>0.4375</v>
       </c>
       <c r="V7" s="8">
         <f t="shared" si="2"/>
-        <v>3.4337276181752696E-2</v>
+        <v>-6.9619213839557936E-3</v>
       </c>
       <c r="W7" s="8">
         <f t="shared" si="4"/>
-        <v>3.5776164329882668E-3</v>
+        <v>-4.0771614211379152E-4</v>
       </c>
       <c r="X7" s="8">
         <f t="shared" si="5"/>
-        <v>-1.1362035392492855E-3</v>
+        <v>4.9943409294691079E-4</v>
       </c>
       <c r="Y7" s="8">
         <f t="shared" si="6"/>
@@ -7185,32 +7253,32 @@
       </c>
       <c r="AB7" s="8">
         <f t="shared" ref="AB7:AB44" si="13">IF(AH6&gt;0,AF6,AB6)</f>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="AC7" s="8">
-        <v>-47.313913459105152</v>
+        <v>-98.697740238587812</v>
       </c>
       <c r="AD7" s="8">
         <f t="shared" ref="AD7:AD44" si="14">IF(AI6&gt;0,AF6,AD6)</f>
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="AE7" s="8">
-        <v>25.674914961811965</v>
+        <v>142.55710353272457</v>
       </c>
       <c r="AF7" s="8">
         <f t="shared" si="9"/>
-        <v>1750</v>
+        <v>1250</v>
       </c>
       <c r="AG7" s="8">
-        <v>-1.3484183383602613</v>
+        <v>24.988074606286091</v>
       </c>
       <c r="AH7" s="8">
         <f t="shared" si="10"/>
-        <v>63.798948567847766</v>
+        <v>-2466.2664965536769</v>
       </c>
       <c r="AI7" s="8">
         <f t="shared" si="11"/>
-        <v>-34.620526170347503</v>
+        <v>3562.2275387317718</v>
       </c>
       <c r="AJ7" s="8">
         <f t="shared" si="12"/>
@@ -7229,7 +7297,7 @@
       </c>
       <c r="G8">
         <f xml:space="preserve"> K23 + K18 * (K28 * K25 + $C$23 * SIN(K17))</f>
-        <v>108255.92346359526</v>
+        <v>48888.096169850709</v>
       </c>
       <c r="H8" t="s">
         <v>35</v>
@@ -7239,7 +7307,7 @@
       </c>
       <c r="K8">
         <f xml:space="preserve"> K5 * $C$24 * K7</f>
-        <v>679.87060816249573</v>
+        <v>526.39169263491567</v>
       </c>
       <c r="L8" t="s">
         <v>37</v>
@@ -7249,35 +7317,35 @@
       </c>
       <c r="Q8" s="8">
         <f t="shared" si="7"/>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
       <c r="R8" s="8">
         <f t="shared" si="0"/>
-        <v>3.4337276181752696E-2</v>
+        <v>5.8563738317039926E-2</v>
       </c>
       <c r="S8" s="8">
         <f t="shared" si="8"/>
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
       <c r="T8" s="8">
         <f t="shared" si="1"/>
-        <v>-3.3089506961332005E-2</v>
+        <v>-6.9619213839557936E-3</v>
       </c>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>0.34375</v>
+        <v>0.40625</v>
       </c>
       <c r="V8" s="8">
         <f t="shared" si="2"/>
-        <v>4.0212566897224189E-4</v>
+        <v>2.5685907249851925E-2</v>
       </c>
       <c r="W8" s="8">
         <f t="shared" si="4"/>
-        <v>1.3807900155271931E-5</v>
+        <v>1.5042627506160868E-3</v>
       </c>
       <c r="X8" s="8">
         <f t="shared" si="5"/>
-        <v>-1.3306140122787288E-5</v>
+        <v>-1.7882326694904926E-4</v>
       </c>
       <c r="Y8" s="8">
         <f t="shared" si="6"/>
@@ -7288,32 +7356,32 @@
       </c>
       <c r="AB8" s="8">
         <f t="shared" si="13"/>
-        <v>1750</v>
+        <v>1000</v>
       </c>
       <c r="AC8" s="8">
-        <v>-1.3484183383602613</v>
+        <v>-98.697740238587812</v>
       </c>
       <c r="AD8" s="8">
         <f t="shared" si="14"/>
-        <v>2000</v>
+        <v>1250</v>
       </c>
       <c r="AE8" s="8">
-        <v>25.674914961811965</v>
+        <v>24.988074606286091</v>
       </c>
       <c r="AF8" s="8">
         <f t="shared" si="9"/>
-        <v>1875</v>
+        <v>1125</v>
       </c>
       <c r="AG8" s="8">
-        <v>14.608622084738727</v>
+        <v>-36.160048462268151</v>
       </c>
       <c r="AH8" s="8">
         <f t="shared" si="10"/>
-        <v>-19.698533917236411</v>
+        <v>3568.9150701436888</v>
       </c>
       <c r="AI8" s="8">
         <f t="shared" si="11"/>
-        <v>375.07512973491504</v>
+        <v>-903.56998874207716</v>
       </c>
       <c r="AJ8" s="8">
         <f t="shared" si="12"/>
@@ -7332,7 +7400,7 @@
       </c>
       <c r="G9">
         <f xml:space="preserve"> $C$6 * G8</f>
-        <v>108255.92346359526</v>
+        <v>48888.096169850709</v>
       </c>
       <c r="H9" t="s">
         <v>35</v>
@@ -7349,35 +7417,35 @@
       </c>
       <c r="Q9" s="8">
         <f t="shared" si="7"/>
-        <v>0.34375</v>
+        <v>0.40625</v>
       </c>
       <c r="R9" s="8">
         <f t="shared" si="0"/>
-        <v>4.0212566897224189E-4</v>
+        <v>2.5685907249851925E-2</v>
       </c>
       <c r="S9" s="8">
         <f t="shared" si="8"/>
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
       <c r="T9" s="8">
         <f t="shared" si="1"/>
-        <v>-3.3089506961332005E-2</v>
+        <v>-6.9619213839557936E-3</v>
       </c>
       <c r="U9" s="8">
         <f t="shared" si="3"/>
-        <v>0.359375</v>
+        <v>0.421875</v>
       </c>
       <c r="V9" s="8">
         <f t="shared" si="2"/>
-        <v>-1.6391988222810072E-2</v>
+        <v>9.3363891812671684E-3</v>
       </c>
       <c r="W9" s="8">
         <f t="shared" si="4"/>
-        <v>-6.5916392298826105E-6</v>
+        <v>2.3981362655854944E-4</v>
       </c>
       <c r="X9" s="8">
         <f t="shared" si="5"/>
-        <v>5.4240280840874607E-4</v>
+        <v>-6.4999207489997425E-5</v>
       </c>
       <c r="Y9" s="8">
         <f t="shared" si="6"/>
@@ -7388,32 +7456,32 @@
       </c>
       <c r="AB9" s="8">
         <f t="shared" si="13"/>
-        <v>1750</v>
+        <v>1125</v>
       </c>
       <c r="AC9" s="8">
-        <v>-1.3484183383602613</v>
+        <v>-36.160048462268151</v>
       </c>
       <c r="AD9" s="8">
         <f t="shared" si="14"/>
-        <v>1875</v>
+        <v>1250</v>
       </c>
       <c r="AE9" s="8">
-        <v>14.608622084738727</v>
+        <v>24.988074606286091</v>
       </c>
       <c r="AF9" s="8">
         <f t="shared" si="9"/>
-        <v>1812.5</v>
+        <v>1187.5</v>
       </c>
       <c r="AG9" s="8">
-        <v>7.2315173400106687</v>
+        <v>-5.4023833145230356</v>
       </c>
       <c r="AH9" s="8">
         <f t="shared" si="10"/>
-        <v>-9.7511105954406023</v>
+        <v>195.35044246490182</v>
       </c>
       <c r="AI9" s="8">
         <f t="shared" si="11"/>
-        <v>105.6425039194509</v>
+        <v>-134.99515731505676</v>
       </c>
       <c r="AJ9" s="8">
         <f t="shared" si="12"/>
@@ -7426,42 +7494,42 @@
       </c>
       <c r="K10">
         <f xml:space="preserve"> K4 / (K5 * $C$24)</f>
-        <v>1.4554294148452218</v>
+        <v>0.59999999994155828</v>
       </c>
       <c r="P10" s="8">
         <v>6</v>
       </c>
       <c r="Q10" s="8">
         <f t="shared" si="7"/>
-        <v>0.34375</v>
+        <v>0.421875</v>
       </c>
       <c r="R10" s="8">
         <f t="shared" si="0"/>
-        <v>4.0212566897224189E-4</v>
+        <v>9.3363891812671684E-3</v>
       </c>
       <c r="S10" s="8">
         <f t="shared" si="8"/>
-        <v>0.359375</v>
+        <v>0.4375</v>
       </c>
       <c r="T10" s="8">
         <f t="shared" si="1"/>
-        <v>-1.6391988222810072E-2</v>
+        <v>-6.9619213839557936E-3</v>
       </c>
       <c r="U10" s="8">
         <f t="shared" si="3"/>
-        <v>0.3515625</v>
+        <v>0.4296875</v>
       </c>
       <c r="V10" s="8">
         <f t="shared" si="2"/>
-        <v>-8.0078008059947803E-3</v>
+        <v>1.181177137633882E-3</v>
       </c>
       <c r="W10" s="8">
         <f t="shared" si="4"/>
-        <v>-3.2201422561071089E-6</v>
+        <v>1.1027929448965097E-5</v>
       </c>
       <c r="X10" s="8">
         <f t="shared" si="5"/>
-        <v>1.3126377650247544E-4</v>
+        <v>-8.2232623727330189E-6</v>
       </c>
       <c r="Y10" s="8">
         <f t="shared" si="6"/>
@@ -7472,32 +7540,32 @@
       </c>
       <c r="AB10" s="8">
         <f t="shared" si="13"/>
-        <v>1750</v>
+        <v>1187.5</v>
       </c>
       <c r="AC10" s="8">
-        <v>-1.3484183383602613</v>
+        <v>-5.4023833145230356</v>
       </c>
       <c r="AD10" s="8">
         <f t="shared" si="14"/>
-        <v>1812.5</v>
+        <v>1250</v>
       </c>
       <c r="AE10" s="8">
-        <v>7.2315173400106687</v>
+        <v>24.988074606286091</v>
       </c>
       <c r="AF10" s="8">
         <f t="shared" si="9"/>
-        <v>1781.25</v>
+        <v>1218.75</v>
       </c>
       <c r="AG10" s="8">
-        <v>3.0906758263029133</v>
+        <v>9.8398576323439784</v>
       </c>
       <c r="AH10" s="8">
         <f t="shared" si="10"/>
-        <v>-4.1675239621136013</v>
+        <v>-53.158682690257251</v>
       </c>
       <c r="AI10" s="8">
         <f t="shared" si="11"/>
-        <v>22.350275830261317</v>
+        <v>245.87909663224494</v>
       </c>
       <c r="AJ10" s="8">
         <f t="shared" si="12"/>
@@ -7508,54 +7576,54 @@
       <c r="B11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
       <c r="F11" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
       <c r="J11" t="s">
         <v>71</v>
       </c>
       <c r="K11">
         <f xml:space="preserve"> K7 + K10^2 / ( PI() * K9 * $C$12 )</f>
-        <v>0.14645043752924147</v>
+        <v>4.2006950064540312E-2</v>
       </c>
       <c r="P11" s="8">
         <v>7</v>
       </c>
       <c r="Q11" s="8">
         <f t="shared" si="7"/>
-        <v>0.34375</v>
+        <v>0.4296875</v>
       </c>
       <c r="R11" s="8">
         <f t="shared" si="0"/>
-        <v>4.0212566897224189E-4</v>
+        <v>1.181177137633882E-3</v>
       </c>
       <c r="S11" s="8">
         <f t="shared" si="8"/>
-        <v>0.3515625</v>
+        <v>0.4375</v>
       </c>
       <c r="T11" s="8">
         <f t="shared" si="1"/>
-        <v>-8.0078008059947803E-3</v>
+        <v>-6.9619213839557936E-3</v>
       </c>
       <c r="U11" s="8">
         <f t="shared" si="3"/>
-        <v>0.34765625</v>
+        <v>0.43359375</v>
       </c>
       <c r="V11" s="8">
         <f t="shared" si="2"/>
-        <v>-3.8061620383744721E-3</v>
+        <v>-2.8918459566564803E-3</v>
       </c>
       <c r="W11" s="8">
         <f t="shared" si="4"/>
-        <v>-1.5305554558980865E-6</v>
+        <v>-3.4157823295616164E-6</v>
       </c>
       <c r="X11" s="8">
         <f t="shared" si="5"/>
-        <v>3.0478987438641834E-5</v>
+        <v>2.013280420475285E-5</v>
       </c>
       <c r="Y11" s="8">
         <f t="shared" si="6"/>
@@ -7566,32 +7634,32 @@
       </c>
       <c r="AB11" s="8">
         <f t="shared" si="13"/>
-        <v>1750</v>
+        <v>1187.5</v>
       </c>
       <c r="AC11" s="8">
-        <v>-1.3484183383602613</v>
+        <v>-5.4023833145230356</v>
       </c>
       <c r="AD11" s="8">
         <f t="shared" si="14"/>
-        <v>1781.25</v>
+        <v>1218.75</v>
       </c>
       <c r="AE11" s="8">
-        <v>3.0906758263029133</v>
+        <v>9.8398576323439784</v>
       </c>
       <c r="AF11" s="8">
         <f t="shared" si="9"/>
-        <v>1765.625</v>
+        <v>1203.125</v>
       </c>
       <c r="AG11" s="8">
-        <v>0.9082583887650344</v>
+        <v>2.2303559250751732</v>
       </c>
       <c r="AH11" s="8">
         <f t="shared" si="10"/>
-        <v>-1.2247122673803159</v>
+        <v>-12.049237635073705</v>
       </c>
       <c r="AI11" s="8">
         <f t="shared" si="11"/>
-        <v>2.8071322461929253</v>
+        <v>21.946384772194559</v>
       </c>
       <c r="AJ11" s="8">
         <f t="shared" si="12"/>
@@ -7610,7 +7678,7 @@
       </c>
       <c r="G12">
         <f xml:space="preserve"> (G4*$C$30 + G9*G13)/3600</f>
-        <v>106725.69199918545</v>
+        <v>35808.600464868803</v>
       </c>
       <c r="H12" t="s">
         <v>43</v>
@@ -7620,7 +7688,7 @@
       </c>
       <c r="K12">
         <f xml:space="preserve"> K5 * K11 * $C$24</f>
-        <v>1736.6092882217458</v>
+        <v>823.18345813489111</v>
       </c>
       <c r="L12" t="s">
         <v>37</v>
@@ -7630,35 +7698,35 @@
       </c>
       <c r="Q12" s="8">
         <f t="shared" si="7"/>
-        <v>0.34375</v>
+        <v>0.4296875</v>
       </c>
       <c r="R12" s="8">
         <f t="shared" si="0"/>
-        <v>4.0212566897224189E-4</v>
+        <v>1.181177137633882E-3</v>
       </c>
       <c r="S12" s="8">
         <f t="shared" si="8"/>
-        <v>0.34765625</v>
+        <v>0.43359375</v>
       </c>
       <c r="T12" s="8">
         <f t="shared" si="1"/>
-        <v>-3.8061620383744721E-3</v>
+        <v>-2.8918459566564803E-3</v>
       </c>
       <c r="U12" s="8">
         <f t="shared" si="3"/>
-        <v>0.345703125</v>
+        <v>0.431640625</v>
       </c>
       <c r="V12" s="8">
         <f t="shared" si="2"/>
-        <v>-1.7028632090883011E-3</v>
+        <v>-8.5570780034160965E-4</v>
       </c>
       <c r="W12" s="8">
         <f t="shared" si="4"/>
-        <v>-6.8476500712285176E-7</v>
+        <v>-1.0107424902584879E-6</v>
       </c>
       <c r="X12" s="8">
         <f t="shared" si="5"/>
-        <v>6.4813733029764234E-6</v>
+        <v>2.4745751424972946E-6</v>
       </c>
       <c r="Y12" s="8">
         <f t="shared" si="6"/>
@@ -7669,32 +7737,32 @@
       </c>
       <c r="AB12" s="8">
         <f t="shared" si="13"/>
-        <v>1750</v>
+        <v>1187.5</v>
       </c>
       <c r="AC12" s="8">
-        <v>-1.3484183383602613</v>
+        <v>-5.4023833145230356</v>
       </c>
       <c r="AD12" s="8">
         <f t="shared" si="14"/>
-        <v>1765.625</v>
+        <v>1203.125</v>
       </c>
       <c r="AE12" s="8">
-        <v>0.9082583887650344</v>
+        <v>2.2303559250751732</v>
       </c>
       <c r="AF12" s="8">
         <f t="shared" si="9"/>
-        <v>1757.8125</v>
+        <v>1195.3125</v>
       </c>
       <c r="AG12" s="8">
-        <v>-0.21081603648985947</v>
+        <v>-1.5831262617477933</v>
       </c>
       <c r="AH12" s="8">
         <f t="shared" si="10"/>
-        <v>0.28426820962335253</v>
+        <v>8.5526549012495057</v>
       </c>
       <c r="AI12" s="8">
         <f t="shared" si="11"/>
-        <v>-0.19147543362811045</v>
+        <v>-3.5309350380313003</v>
       </c>
       <c r="AJ12" s="8">
         <f t="shared" si="12"/>
@@ -7707,45 +7775,52 @@
       </c>
       <c r="G13">
         <f xml:space="preserve"> $C$29 / $C$23</f>
-        <v>2727.2727272727275</v>
+        <v>1818.1818181818446</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
+      <c r="J13" t="s">
+        <v>138</v>
+      </c>
+      <c r="K13">
+        <f>K10/K11</f>
+        <v>14.28335070791158</v>
+      </c>
       <c r="P13" s="8">
         <v>9</v>
       </c>
       <c r="Q13" s="8">
         <f t="shared" si="7"/>
-        <v>0.34375</v>
+        <v>0.4296875</v>
       </c>
       <c r="R13" s="8">
         <f t="shared" si="0"/>
-        <v>4.0212566897224189E-4</v>
+        <v>1.181177137633882E-3</v>
       </c>
       <c r="S13" s="8">
         <f t="shared" si="8"/>
-        <v>0.345703125</v>
+        <v>0.431640625</v>
       </c>
       <c r="T13" s="8">
         <f t="shared" si="1"/>
-        <v>-1.7028632090883011E-3</v>
+        <v>-8.5570780034160965E-4</v>
       </c>
       <c r="U13" s="8">
         <f t="shared" si="3"/>
-        <v>0.3447265625</v>
+        <v>0.4306640625</v>
       </c>
       <c r="V13" s="8">
         <f t="shared" si="2"/>
-        <v>-6.5058179843768826E-4</v>
+        <v>1.6264069476540355E-4</v>
       </c>
       <c r="W13" s="8">
         <f t="shared" si="4"/>
-        <v>-2.6161564091791965E-7</v>
+        <v>1.9210747030578525E-7</v>
       </c>
       <c r="X13" s="8">
         <f t="shared" si="5"/>
-        <v>1.1078518090620401E-6</v>
+        <v>-1.3917291116373461E-7</v>
       </c>
       <c r="Y13" s="8">
         <f t="shared" si="6"/>
@@ -7756,32 +7831,32 @@
       </c>
       <c r="AB13" s="8">
         <f t="shared" si="13"/>
-        <v>1757.8125</v>
+        <v>1195.3125</v>
       </c>
       <c r="AC13" s="8">
-        <v>-0.21081603648985947</v>
+        <v>-1.5831262617477933</v>
       </c>
       <c r="AD13" s="8">
         <f t="shared" si="14"/>
-        <v>1765.625</v>
+        <v>1203.125</v>
       </c>
       <c r="AE13" s="8">
-        <v>0.9082583887650344</v>
+        <v>2.2303559250751732</v>
       </c>
       <c r="AF13" s="8">
         <f t="shared" si="9"/>
-        <v>1761.71875</v>
+        <v>1199.21875</v>
       </c>
       <c r="AG13" s="8">
-        <v>0.35103858905245033</v>
+        <v>0.32433894758037241</v>
       </c>
       <c r="AH13" s="8">
         <f t="shared" si="10"/>
-        <v>-7.400456399903016E-2</v>
+        <v>-0.51346950562212845</v>
       </c>
       <c r="AI13" s="8">
         <f t="shared" si="11"/>
-        <v>0.3188337432871296</v>
+        <v>0.72339129346852959</v>
       </c>
       <c r="AJ13" s="8">
         <f t="shared" si="12"/>
@@ -7792,42 +7867,42 @@
       <c r="B14" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
       <c r="P14" s="8">
         <v>10</v>
       </c>
       <c r="Q14" s="8">
         <f t="shared" si="7"/>
-        <v>0.34375</v>
+        <v>0.4306640625</v>
       </c>
       <c r="R14" s="8">
         <f t="shared" si="0"/>
-        <v>4.0212566897224189E-4</v>
+        <v>1.6264069476540355E-4</v>
       </c>
       <c r="S14" s="8">
         <f t="shared" si="8"/>
-        <v>0.3447265625</v>
+        <v>0.431640625</v>
       </c>
       <c r="T14" s="8">
         <f t="shared" si="1"/>
-        <v>-6.5058179843768826E-4</v>
+        <v>-8.5570780034160965E-4</v>
       </c>
       <c r="U14" s="8">
         <f t="shared" si="3"/>
-        <v>0.34423828125</v>
+        <v>0.43115234375</v>
       </c>
       <c r="V14" s="8">
         <f t="shared" si="2"/>
-        <v>-1.2428154552712734E-4</v>
+        <v>-3.4655696755120369E-4</v>
       </c>
       <c r="W14" s="8">
         <f t="shared" si="4"/>
-        <v>-4.9976799636000218E-8</v>
+        <v>-5.6364265978319179E-8</v>
       </c>
       <c r="X14" s="8">
         <f t="shared" si="5"/>
-        <v>8.0855311401653939E-8</v>
+        <v>2.9655150039629911E-7</v>
       </c>
       <c r="Y14" s="8">
         <f t="shared" si="6"/>
@@ -7838,32 +7913,32 @@
       </c>
       <c r="AB14" s="8">
         <f t="shared" si="13"/>
-        <v>1757.8125</v>
+        <v>1195.3125</v>
       </c>
       <c r="AC14" s="8">
-        <v>-0.21081603648985947</v>
+        <v>-1.5831262617477933</v>
       </c>
       <c r="AD14" s="8">
         <f t="shared" si="14"/>
-        <v>1761.71875</v>
+        <v>1199.21875</v>
       </c>
       <c r="AE14" s="8">
-        <v>0.35103858905245033</v>
+        <v>0.32433894758037241</v>
       </c>
       <c r="AF14" s="8">
         <f t="shared" si="9"/>
-        <v>1759.765625</v>
+        <v>1197.265625</v>
       </c>
       <c r="AG14" s="8">
-        <v>7.0689910544615486E-2</v>
+        <v>-0.62921274287998585</v>
       </c>
       <c r="AH14" s="8">
         <f t="shared" si="10"/>
-        <v>-1.490256676083856E-2</v>
+        <v>0.99612321747966737</v>
       </c>
       <c r="AI14" s="8">
         <f t="shared" si="11"/>
-        <v>2.4814886457825751E-2</v>
+        <v>-0.20407819882985406</v>
       </c>
       <c r="AJ14" s="8">
         <f t="shared" si="12"/>
@@ -7885,35 +7960,35 @@
       </c>
       <c r="Q15" s="8">
         <f t="shared" si="7"/>
-        <v>0.34375</v>
+        <v>0.4306640625</v>
       </c>
       <c r="R15" s="8">
         <f t="shared" si="0"/>
-        <v>4.0212566897224189E-4</v>
+        <v>1.6264069476540355E-4</v>
       </c>
       <c r="S15" s="8">
         <f t="shared" si="8"/>
-        <v>0.34423828125</v>
+        <v>0.43115234375</v>
       </c>
       <c r="T15" s="8">
         <f t="shared" si="1"/>
-        <v>-1.2428154552712734E-4</v>
+        <v>-3.4655696755120369E-4</v>
       </c>
       <c r="U15" s="8">
         <f t="shared" si="3"/>
-        <v>0.343994140625</v>
+        <v>0.430908203125</v>
       </c>
       <c r="V15" s="8">
         <f t="shared" si="2"/>
-        <v>1.3890866342486374E-4</v>
+        <v>-9.196399989463977E-5</v>
       </c>
       <c r="W15" s="8">
         <f t="shared" si="4"/>
-        <v>5.5858739205763325E-8</v>
+        <v>-1.4957088836269711E-8</v>
       </c>
       <c r="X15" s="8">
         <f t="shared" si="5"/>
-        <v>-1.7263783377549612E-8</v>
+        <v>3.1870764927365571E-8</v>
       </c>
       <c r="Y15" s="8">
         <f t="shared" si="6"/>
@@ -7924,32 +7999,32 @@
       </c>
       <c r="AB15" s="8">
         <f t="shared" si="13"/>
-        <v>1757.8125</v>
+        <v>1197.265625</v>
       </c>
       <c r="AC15" s="8">
-        <v>-0.21081603648985947</v>
+        <v>-0.62921274287998585</v>
       </c>
       <c r="AD15" s="8">
         <f t="shared" si="14"/>
-        <v>1759.765625</v>
+        <v>1199.21875</v>
       </c>
       <c r="AE15" s="8">
-        <v>7.0689910544615486E-2</v>
+        <v>0.32433894758037241</v>
       </c>
       <c r="AF15" s="8">
         <f t="shared" si="9"/>
-        <v>1758.7890625</v>
+        <v>1198.2421875</v>
       </c>
       <c r="AG15" s="8">
-        <v>-6.9918236420789981E-2</v>
+        <v>-0.1523916866287891</v>
       </c>
       <c r="AH15" s="8">
         <f t="shared" si="10"/>
-        <v>1.4739885480591882E-2</v>
+        <v>9.5886791135807656E-2</v>
       </c>
       <c r="AI15" s="8">
         <f t="shared" si="11"/>
-        <v>-4.9425138780229199E-3</v>
+        <v>-4.9426559261179365E-2</v>
       </c>
       <c r="AJ15" s="8">
         <f t="shared" si="12"/>
@@ -7971,42 +8046,42 @@
       <c r="J16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
       <c r="P16" s="8">
         <v>12</v>
       </c>
       <c r="Q16" s="8">
         <f t="shared" si="7"/>
-        <v>0.343994140625</v>
+        <v>0.4306640625</v>
       </c>
       <c r="R16" s="8">
         <f t="shared" si="0"/>
-        <v>1.3890866342486374E-4</v>
+        <v>1.6264069476540355E-4</v>
       </c>
       <c r="S16" s="8">
         <f t="shared" si="8"/>
-        <v>0.34423828125</v>
+        <v>0.430908203125</v>
       </c>
       <c r="T16" s="8">
         <f t="shared" si="1"/>
-        <v>-1.2428154552712734E-4</v>
+        <v>-9.196399989463977E-5</v>
       </c>
       <c r="U16" s="8">
         <f t="shared" si="3"/>
-        <v>0.3441162109375</v>
+        <v>0.4307861328125</v>
       </c>
       <c r="V16" s="8">
         <f t="shared" si="2"/>
-        <v>7.3102128929636301E-6</v>
+        <v>3.5336880331138243E-5</v>
       </c>
       <c r="W16" s="8">
         <f t="shared" si="4"/>
-        <v>1.0154519023127844E-9</v>
+        <v>5.747214767898247E-9</v>
       </c>
       <c r="X16" s="8">
         <f t="shared" si="5"/>
-        <v>-9.085245564698526E-10</v>
+        <v>-3.2497208590496955E-9</v>
       </c>
       <c r="Y16" s="8">
         <f t="shared" si="6"/>
@@ -8017,32 +8092,32 @@
       </c>
       <c r="AB16" s="8">
         <f t="shared" si="13"/>
-        <v>1758.7890625</v>
+        <v>1198.2421875</v>
       </c>
       <c r="AC16" s="8">
-        <v>-6.9918236420789981E-2</v>
+        <v>-0.1523916866287891</v>
       </c>
       <c r="AD16" s="8">
         <f t="shared" si="14"/>
-        <v>1759.765625</v>
+        <v>1199.21875</v>
       </c>
       <c r="AE16" s="8">
-        <v>7.0689910544615486E-2</v>
+        <v>0.32433894758037241</v>
       </c>
       <c r="AF16" s="8">
         <f t="shared" si="9"/>
-        <v>1759.27734375</v>
+        <v>1198.73046875</v>
       </c>
       <c r="AG16" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>8.5984834820919787E-2</v>
       </c>
       <c r="AH16" s="8">
         <f t="shared" si="10"/>
-        <v>-2.952329775813371E-5</v>
+        <v>-1.3103374002857802E-2</v>
       </c>
       <c r="AI16" s="8">
         <f t="shared" si="11"/>
-        <v>2.9849140715510894E-5</v>
+        <v>2.7888230833689284E-2</v>
       </c>
       <c r="AJ16" s="8">
         <f t="shared" si="12"/>
@@ -8061,7 +8136,7 @@
       </c>
       <c r="G17">
         <f xml:space="preserve"> G12 / ($C$15 * $C$16 * $C$17)</f>
-        <v>627.79818823050266</v>
+        <v>210.63882626393413</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
@@ -8081,35 +8156,35 @@
       </c>
       <c r="Q17" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441162109375</v>
+        <v>0.4307861328125</v>
       </c>
       <c r="R17" s="8">
         <f t="shared" si="0"/>
-        <v>7.3102128929636301E-6</v>
+        <v>3.5336880331138243E-5</v>
       </c>
       <c r="S17" s="8">
         <f t="shared" si="8"/>
-        <v>0.34423828125</v>
+        <v>0.430908203125</v>
       </c>
       <c r="T17" s="8">
         <f t="shared" si="1"/>
-        <v>-1.2428154552712734E-4</v>
+        <v>-9.196399989463977E-5</v>
       </c>
       <c r="U17" s="8">
         <f t="shared" si="3"/>
-        <v>0.34417724609375</v>
+        <v>0.43084716796875</v>
       </c>
       <c r="V17" s="8">
         <f t="shared" si="2"/>
-        <v>-5.8486502391763562E-5</v>
+        <v>-2.8313926404122114E-5</v>
       </c>
       <c r="W17" s="8">
         <f t="shared" si="4"/>
-        <v>-4.275487838486182E-10</v>
+        <v>-1.0005258290471184E-9</v>
       </c>
       <c r="X17" s="8">
         <f t="shared" si="5"/>
-        <v>7.2687929097244045E-9</v>
+        <v>2.6038619248455244E-9</v>
       </c>
       <c r="Y17" s="8">
         <f t="shared" si="6"/>
@@ -8120,32 +8195,32 @@
       </c>
       <c r="AB17" s="8">
         <f t="shared" si="13"/>
-        <v>1758.7890625</v>
+        <v>1198.2421875</v>
       </c>
       <c r="AC17" s="8">
-        <v>-6.9918236420789981E-2</v>
+        <v>-0.1523916866287891</v>
       </c>
       <c r="AD17" s="8">
         <f t="shared" si="14"/>
-        <v>1759.27734375</v>
+        <v>1198.73046875</v>
       </c>
       <c r="AE17" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>8.5984834820919787E-2</v>
       </c>
       <c r="AF17" s="8">
         <f t="shared" si="9"/>
-        <v>1759.033203125</v>
+        <v>1198.486328125</v>
       </c>
       <c r="AG17" s="8">
-        <v>-3.4738475067570107E-2</v>
+        <v>-3.32006766085442E-2</v>
       </c>
       <c r="AH17" s="8">
         <f t="shared" si="10"/>
-        <v>2.4288529126720851E-3</v>
+        <v>5.0595071055930365E-3</v>
       </c>
       <c r="AI17" s="8">
         <f t="shared" si="11"/>
-        <v>-1.4668481294508436E-5</v>
+        <v>-2.8547546941284484E-3</v>
       </c>
       <c r="AJ17" s="8">
         <f t="shared" si="12"/>
@@ -8158,7 +8233,7 @@
       </c>
       <c r="G18">
         <f xml:space="preserve"> $C$5 * 0.144 * (2*$C$21*3.28084 * (G4*0.00134102/$C$5) * 4^0.5)^0.782 * 0.453592 + C6 * $C$6 * 0.144 * (2*$C$22*3.28084 * (G9*0.00134102/$C$6) * 4^0.5)^0.782 * 0.453592</f>
-        <v>129.12379999708568</v>
+        <v>79.76666441523615</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
@@ -8168,7 +8243,7 @@
       </c>
       <c r="K18">
         <f xml:space="preserve"> K12 / $C$6</f>
-        <v>1736.6092882217458</v>
+        <v>823.18345813489111</v>
       </c>
       <c r="L18" t="s">
         <v>37</v>
@@ -8178,35 +8253,35 @@
       </c>
       <c r="Q18" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441162109375</v>
+        <v>0.4307861328125</v>
       </c>
       <c r="R18" s="8">
         <f t="shared" si="0"/>
-        <v>7.3102128929636301E-6</v>
+        <v>3.5336880331138243E-5</v>
       </c>
       <c r="S18" s="8">
         <f t="shared" si="8"/>
-        <v>0.34417724609375</v>
+        <v>0.43084716796875</v>
       </c>
       <c r="T18" s="8">
         <f t="shared" si="1"/>
-        <v>-5.8486502391763562E-5</v>
+        <v>-2.8313926404122114E-5</v>
       </c>
       <c r="U18" s="8">
         <f t="shared" si="3"/>
-        <v>0.344146728515625</v>
+        <v>0.430816650390625</v>
       </c>
       <c r="V18" s="8">
         <f t="shared" si="2"/>
-        <v>-2.5588353822936227E-5</v>
+        <v>3.5113852887569408E-6</v>
       </c>
       <c r="W18" s="8">
         <f t="shared" si="4"/>
-        <v>-1.8705631402614359E-10</v>
+        <v>1.2408140174532331E-10</v>
       </c>
       <c r="X18" s="8">
         <f t="shared" si="5"/>
-        <v>1.496573317066452E-9</v>
+        <v>-9.9421104642381105E-11</v>
       </c>
       <c r="Y18" s="8">
         <f t="shared" si="6"/>
@@ -8217,32 +8292,32 @@
       </c>
       <c r="AB18" s="8">
         <f t="shared" si="13"/>
-        <v>1759.033203125</v>
+        <v>1198.486328125</v>
       </c>
       <c r="AC18" s="8">
-        <v>-3.4738475067570107E-2</v>
+        <v>-3.32006766085442E-2</v>
       </c>
       <c r="AD18" s="8">
         <f t="shared" si="14"/>
-        <v>1759.27734375</v>
+        <v>1198.73046875</v>
       </c>
       <c r="AE18" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>8.5984834820919787E-2</v>
       </c>
       <c r="AF18" s="8">
         <f t="shared" si="9"/>
-        <v>1759.1552734375</v>
+        <v>1198.6083984375</v>
       </c>
       <c r="AG18" s="8">
-        <v>-1.7156761490696226E-2</v>
+        <v>2.6392766487902009E-2</v>
       </c>
       <c r="AH18" s="8">
         <f t="shared" si="10"/>
-        <v>5.9599973128479785E-4</v>
+        <v>-8.7625770496965749E-4</v>
       </c>
       <c r="AI18" s="8">
         <f t="shared" si="11"/>
-        <v>-7.2445216582221059E-6</v>
+        <v>2.2693776669293615E-3</v>
       </c>
       <c r="AJ18" s="8">
         <f t="shared" si="12"/>
@@ -8250,17 +8325,17 @@
       </c>
     </row>
     <row r="19" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="F19" s="13" t="s">
         <v>89</v>
       </c>
       <c r="G19">
         <f xml:space="preserve"> 0.188 * (G4/1000) + 5.836 + 0.188 * (G9/1000) + 5.836</f>
-        <v>101.71654674026901</v>
+        <v>52.214714785316005</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
@@ -8270,7 +8345,7 @@
       </c>
       <c r="K19">
         <f xml:space="preserve"> PI() * $C$23 / ($C$22 * $C$25)</f>
-        <v>191.98621771937624</v>
+        <v>153.14932077647677</v>
       </c>
       <c r="L19" t="s">
         <v>54</v>
@@ -8280,35 +8355,35 @@
       </c>
       <c r="Q19" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441162109375</v>
+        <v>0.430816650390625</v>
       </c>
       <c r="R19" s="8">
         <f t="shared" si="0"/>
-        <v>7.3102128929636301E-6</v>
+        <v>3.5113852887569408E-6</v>
       </c>
       <c r="S19" s="8">
         <f t="shared" si="8"/>
-        <v>0.344146728515625</v>
+        <v>0.43084716796875</v>
       </c>
       <c r="T19" s="8">
         <f t="shared" si="1"/>
-        <v>-2.5588353822936227E-5</v>
+        <v>-2.8313926404122114E-5</v>
       </c>
       <c r="U19" s="8">
         <f t="shared" si="3"/>
-        <v>0.3441314697265625</v>
+        <v>0.4308319091796875</v>
       </c>
       <c r="V19" s="8">
         <f t="shared" si="2"/>
-        <v>-9.1391227402537467E-6</v>
+        <v>-1.2401293473962571E-5</v>
       </c>
       <c r="W19" s="8">
         <f t="shared" si="4"/>
-        <v>-6.6808932886180036E-11</v>
+        <v>-4.3545719466029626E-11</v>
       </c>
       <c r="X19" s="8">
         <f t="shared" si="5"/>
-        <v>2.3385510630885535E-10</v>
+        <v>3.5112931073769609E-10</v>
       </c>
       <c r="Y19" s="8">
         <f t="shared" si="6"/>
@@ -8319,32 +8394,32 @@
       </c>
       <c r="AB19" s="8">
         <f t="shared" si="13"/>
-        <v>1759.1552734375</v>
+        <v>1198.486328125</v>
       </c>
       <c r="AC19" s="8">
-        <v>-1.7156761490696226E-2</v>
+        <v>-3.32006766085442E-2</v>
       </c>
       <c r="AD19" s="8">
         <f t="shared" si="14"/>
-        <v>1759.27734375</v>
+        <v>1198.6083984375</v>
       </c>
       <c r="AE19" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>2.6392766487902009E-2</v>
       </c>
       <c r="AF19" s="8">
         <f t="shared" si="9"/>
-        <v>1759.21630859375</v>
+        <v>1198.54736328125</v>
       </c>
       <c r="AG19" s="8">
-        <v>-8.3667102057916054E-3</v>
+        <v>-3.4035780588510534E-3</v>
       </c>
       <c r="AH19" s="8">
         <f t="shared" si="10"/>
-        <v>1.4354565146254051E-4</v>
+        <v>1.1300109444385044E-4</v>
       </c>
       <c r="AI19" s="8">
         <f t="shared" si="11"/>
-        <v>-3.5328819676600593E-6</v>
+        <v>-8.9829840930602656E-5</v>
       </c>
       <c r="AJ19" s="8">
         <f t="shared" si="12"/>
@@ -8357,7 +8432,7 @@
       </c>
       <c r="C20" s="3">
         <f>AF44</f>
-        <v>1759.2744139892602</v>
+        <v>1198.5543353202956</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>14</v>
@@ -8367,7 +8442,7 @@
       </c>
       <c r="G20">
         <f xml:space="preserve"> 14.86 * ($C$20*2.20462)^0.144 * (6.7/(PI()*1.8))^0.778 * (6.7*3.28084)^0.383 * 4^0.455 * 0.453592</f>
-        <v>155.13153788682038</v>
+        <v>146.79077861950864</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
@@ -8377,42 +8452,42 @@
       </c>
       <c r="K20">
         <f xml:space="preserve"> $C$23 * COS(K17) / (K19 * $C$22)</f>
-        <v>2.7742534554270872E-2</v>
+        <v>3.6065294920551015E-2</v>
       </c>
       <c r="P20" s="8">
         <v>16</v>
       </c>
       <c r="Q20" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441162109375</v>
+        <v>0.430816650390625</v>
       </c>
       <c r="R20" s="8">
         <f t="shared" si="0"/>
-        <v>7.3102128929636301E-6</v>
+        <v>3.5113852887569408E-6</v>
       </c>
       <c r="S20" s="8">
         <f t="shared" si="8"/>
-        <v>0.3441314697265625</v>
+        <v>0.4308319091796875</v>
       </c>
       <c r="T20" s="8">
         <f t="shared" si="1"/>
-        <v>-9.1391227402537467E-6</v>
+        <v>-1.2401293473962571E-5</v>
       </c>
       <c r="U20" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412384033203125</v>
+        <v>0.43082427978515625</v>
       </c>
       <c r="V20" s="8">
         <f t="shared" si="2"/>
-        <v>-9.1446799327377093E-7</v>
+        <v>-4.4449598219920006E-6</v>
       </c>
       <c r="W20" s="8">
         <f t="shared" si="4"/>
-        <v>-6.684955714632498E-12</v>
+        <v>-1.5607966528058381E-11</v>
       </c>
       <c r="X20" s="8">
         <f t="shared" si="5"/>
-        <v>8.3574352325625303E-12</v>
+        <v>5.512325123249523E-11</v>
       </c>
       <c r="Y20" s="8">
         <f t="shared" si="6"/>
@@ -8423,32 +8498,32 @@
       </c>
       <c r="AB20" s="8">
         <f t="shared" si="13"/>
-        <v>1759.21630859375</v>
+        <v>1198.54736328125</v>
       </c>
       <c r="AC20" s="8">
-        <v>-8.3667102057916054E-3</v>
+        <v>-3.4035780588510534E-3</v>
       </c>
       <c r="AD20" s="8">
         <f t="shared" si="14"/>
-        <v>1759.27734375</v>
+        <v>1198.6083984375</v>
       </c>
       <c r="AE20" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>2.6392766487902009E-2</v>
       </c>
       <c r="AF20" s="8">
         <f t="shared" si="9"/>
-        <v>1759.246826171875</v>
+        <v>1198.577880859375</v>
       </c>
       <c r="AG20" s="8">
-        <v>-3.9720919878618588E-3</v>
+        <v>1.1494842348497514E-2</v>
       </c>
       <c r="AH20" s="8">
         <f t="shared" si="10"/>
-        <v>3.3233342573186878E-5</v>
+        <v>-3.9123593207298053E-5</v>
       </c>
       <c r="AI20" s="8">
         <f t="shared" si="11"/>
-        <v>-1.6772341592625357E-6</v>
+        <v>3.0338068991914201E-4</v>
       </c>
       <c r="AJ20" s="8">
         <f t="shared" si="12"/>
@@ -8460,7 +8535,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="1">
-        <v>1.2</v>
+        <v>1.49999999999999</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>
@@ -8470,7 +8545,7 @@
       </c>
       <c r="G21">
         <f xml:space="preserve"> 0.054 * (0.7*3.28084)^0.501 * ($C$20*2.20462*5.7)^0.684 * 0.453592</f>
-        <v>34.803957488997163</v>
+        <v>26.768395583058929</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
@@ -8480,42 +8555,42 @@
       </c>
       <c r="K21">
         <f xml:space="preserve"> K18 / ( $C$33 * PI() * $C$22^2 * K19^2 * $C$22^2)</f>
-        <v>1.8659758335729235E-2</v>
+        <v>1.6075481273085567E-2</v>
       </c>
       <c r="P21" s="8">
         <v>17</v>
       </c>
       <c r="Q21" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441162109375</v>
+        <v>0.430816650390625</v>
       </c>
       <c r="R21" s="8">
         <f t="shared" si="0"/>
-        <v>7.3102128929636301E-6</v>
+        <v>3.5113852887569408E-6</v>
       </c>
       <c r="S21" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412384033203125</v>
+        <v>0.43082427978515625</v>
       </c>
       <c r="T21" s="8">
         <f t="shared" si="1"/>
-        <v>-9.1446799327377093E-7</v>
+        <v>-4.4449598219920006E-6</v>
       </c>
       <c r="U21" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412002563476562</v>
+        <v>0.43082046508789062</v>
       </c>
       <c r="V21" s="8">
         <f t="shared" si="2"/>
-        <v>3.1978691823475458E-6</v>
+        <v>-4.6678869902727627E-7</v>
       </c>
       <c r="W21" s="8">
         <f t="shared" si="4"/>
-        <v>2.337710452680809E-11</v>
+        <v>-1.6390749707223692E-12</v>
       </c>
       <c r="X21" s="8">
         <f t="shared" si="5"/>
-        <v>-2.9243490139333949E-12</v>
+        <v>2.0748570125361595E-12</v>
       </c>
       <c r="Y21" s="8">
         <f t="shared" si="6"/>
@@ -8526,32 +8601,32 @@
       </c>
       <c r="AB21" s="8">
         <f t="shared" si="13"/>
-        <v>1759.246826171875</v>
+        <v>1198.54736328125</v>
       </c>
       <c r="AC21" s="8">
-        <v>-3.9720919878618588E-3</v>
+        <v>-3.4035780588510534E-3</v>
       </c>
       <c r="AD21" s="8">
         <f t="shared" si="14"/>
-        <v>1759.27734375</v>
+        <v>1198.577880859375</v>
       </c>
       <c r="AE21" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>1.1494842348497514E-2</v>
       </c>
       <c r="AF21" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2620849609375</v>
+        <v>1198.5626220703125</v>
       </c>
       <c r="AG21" s="8">
-        <v>-1.774884736050808E-3</v>
+        <v>4.0454377171954548E-3</v>
       </c>
       <c r="AH21" s="8">
         <f t="shared" si="10"/>
-        <v>7.0500054394457242E-6</v>
+        <v>-1.3768963052694943E-5</v>
       </c>
       <c r="AI21" s="8">
         <f t="shared" si="11"/>
-        <v>-7.494532647166919E-7</v>
+        <v>4.650166878982742E-5</v>
       </c>
       <c r="AJ21" s="8">
         <f t="shared" si="12"/>
@@ -8563,7 +8638,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="1">
-        <v>0.9</v>
+        <v>0.86786891819242595</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
@@ -8573,7 +8648,7 @@
       </c>
       <c r="G22">
         <f xml:space="preserve"> 0.04674 * ($C$20*2.20462)^0.397 * ($C$24*3.28084^2)^0.36 * 3^0.397 * $C$12^1.712 * 0.453592</f>
-        <v>206.16084700286123</v>
+        <v>212.1167319418031</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
@@ -8589,35 +8664,35 @@
       </c>
       <c r="Q22" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412002563476562</v>
+        <v>0.430816650390625</v>
       </c>
       <c r="R22" s="8">
         <f t="shared" si="0"/>
-        <v>3.1978691823475458E-6</v>
+        <v>3.5113852887569408E-6</v>
       </c>
       <c r="S22" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412384033203125</v>
+        <v>0.43082046508789062</v>
       </c>
       <c r="T22" s="8">
         <f t="shared" si="1"/>
-        <v>-9.1446799327377093E-7</v>
+        <v>-4.6678869902727627E-7</v>
       </c>
       <c r="U22" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412193298339844</v>
+        <v>0.43081855773925781</v>
       </c>
       <c r="V22" s="8">
         <f t="shared" si="2"/>
-        <v>1.1416997776625415E-6</v>
+        <v>1.5222979367623957E-6</v>
       </c>
       <c r="W22" s="8">
         <f t="shared" si="4"/>
-        <v>3.6510065344800862E-12</v>
+        <v>5.3453745802525202E-12</v>
       </c>
       <c r="X22" s="8">
         <f t="shared" si="5"/>
-        <v>-1.0440479046001747E-12</v>
+        <v>-7.1059147343322556E-13</v>
       </c>
       <c r="Y22" s="8">
         <f t="shared" si="6"/>
@@ -8628,32 +8703,32 @@
       </c>
       <c r="AB22" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2620849609375</v>
+        <v>1198.54736328125</v>
       </c>
       <c r="AC22" s="8">
-        <v>-1.774884736050808E-3</v>
+        <v>-3.4035780588510534E-3</v>
       </c>
       <c r="AD22" s="8">
         <f t="shared" si="14"/>
-        <v>1759.27734375</v>
+        <v>1198.5626220703125</v>
       </c>
       <c r="AE22" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>4.0454377171954548E-3</v>
       </c>
       <c r="AF22" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2697143554688</v>
+        <v>1198.5549926757812</v>
       </c>
       <c r="AG22" s="8">
-        <v>-6.7548221659308183E-4</v>
+        <v>3.2093251491005503E-4</v>
       </c>
       <c r="AH22" s="8">
         <f t="shared" si="10"/>
-        <v>1.1989030757048268E-6</v>
+        <v>-1.0923188661197518E-6</v>
       </c>
       <c r="AI22" s="8">
         <f t="shared" si="11"/>
-        <v>-2.8522548095723832E-7</v>
+        <v>1.2983125004915294E-6</v>
       </c>
       <c r="AJ22" s="8">
         <f t="shared" si="12"/>
@@ -8665,7 +8740,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="1">
-        <v>55</v>
+        <v>54.999999999999197</v>
       </c>
       <c r="D23" t="s">
         <v>19</v>
@@ -8684,7 +8759,7 @@
       </c>
       <c r="K23">
         <f xml:space="preserve"> ($C$8 * $K$22 / 8) * (1 + 4.65 * K20^2) * ( PI() * $C$33 * K19^3 * C22^5)</f>
-        <v>3146.9858091218234</v>
+        <v>1335.2275825919908</v>
       </c>
       <c r="L23" t="s">
         <v>35</v>
@@ -8694,35 +8769,35 @@
       </c>
       <c r="Q23" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412193298339844</v>
+        <v>0.43081855773925781</v>
       </c>
       <c r="R23" s="8">
         <f t="shared" si="0"/>
-        <v>1.1416997776625415E-6</v>
+        <v>1.5222979367623957E-6</v>
       </c>
       <c r="S23" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412384033203125</v>
+        <v>0.43082046508789062</v>
       </c>
       <c r="T23" s="8">
         <f t="shared" si="1"/>
-        <v>-9.1446799327377093E-7</v>
+        <v>-4.6678869902727627E-7</v>
       </c>
       <c r="U23" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412288665771484</v>
+        <v>0.43081951141357422</v>
       </c>
       <c r="V23" s="8">
         <f t="shared" si="2"/>
-        <v>1.136156879688599E-7</v>
+        <v>5.2775452935582834E-7</v>
       </c>
       <c r="W23" s="8">
         <f t="shared" si="4"/>
-        <v>1.2971500569302404E-13</v>
+        <v>8.0339963115538665E-13</v>
       </c>
       <c r="X23" s="8">
         <f t="shared" si="5"/>
-        <v>-1.0389791018130224E-13</v>
+        <v>-2.4634985016375957E-13</v>
       </c>
       <c r="Y23" s="8">
         <f t="shared" si="6"/>
@@ -8733,32 +8808,32 @@
       </c>
       <c r="AB23" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2697143554688</v>
+        <v>1198.54736328125</v>
       </c>
       <c r="AC23" s="8">
-        <v>-6.7548221659308183E-4</v>
+        <v>-3.4035780588510534E-3</v>
       </c>
       <c r="AD23" s="8">
         <f t="shared" si="14"/>
-        <v>1759.27734375</v>
+        <v>1198.5549926757812</v>
       </c>
       <c r="AE23" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>3.2093251491005503E-4</v>
       </c>
       <c r="AF23" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2735290527344</v>
+        <v>1198.5511779785156</v>
       </c>
       <c r="AG23" s="8">
-        <v>-1.2743603952003468E-4</v>
+        <v>-1.5413221004791922E-3</v>
       </c>
       <c r="AH23" s="8">
         <f t="shared" si="10"/>
-        <v>8.6080778448836608E-8</v>
+        <v>5.2460100828131967E-6</v>
       </c>
       <c r="AI23" s="8">
         <f t="shared" si="11"/>
-        <v>-5.3810455361379228E-8</v>
+        <v>-4.9466037799323565E-7</v>
       </c>
       <c r="AJ23" s="8">
         <f t="shared" si="12"/>
@@ -8770,7 +8845,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="1">
-        <v>6.4</v>
+        <v>10.576549642446899</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
@@ -8789,42 +8864,42 @@
       </c>
       <c r="K24" s="5">
         <f>U34</f>
-        <v>0.34412299236282706</v>
+        <v>0.43082001758739352</v>
       </c>
       <c r="P24" s="8">
         <v>20</v>
       </c>
       <c r="Q24" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412288665771484</v>
+        <v>0.43081951141357422</v>
       </c>
       <c r="R24" s="8">
         <f t="shared" si="0"/>
-        <v>1.136156879688599E-7</v>
+        <v>5.2775452935582834E-7</v>
       </c>
       <c r="S24" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412384033203125</v>
+        <v>0.43082046508789062</v>
       </c>
       <c r="T24" s="8">
         <f t="shared" si="1"/>
-        <v>-9.1446799327377093E-7</v>
+        <v>-4.6678869902727627E-7</v>
       </c>
       <c r="U24" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412336349487305</v>
+        <v>0.43081998825073242</v>
       </c>
       <c r="V24" s="8">
         <f t="shared" si="2"/>
-        <v>-4.0042620375047022E-7</v>
+        <v>3.0482892765526515E-8</v>
       </c>
       <c r="W24" s="8">
         <f t="shared" si="4"/>
-        <v>-4.5494698619868544E-14</v>
+        <v>1.6087484724874629E-14</v>
       </c>
       <c r="X24" s="8">
         <f t="shared" si="5"/>
-        <v>3.6617694699792661E-13</v>
+        <v>-1.4229069856608094E-14</v>
       </c>
       <c r="Y24" s="8">
         <f t="shared" si="6"/>
@@ -8835,32 +8910,32 @@
       </c>
       <c r="AB24" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2735290527344</v>
+        <v>1198.5511779785156</v>
       </c>
       <c r="AC24" s="8">
-        <v>-1.2743603952003468E-4</v>
+        <v>-1.5413221004791922E-3</v>
       </c>
       <c r="AD24" s="8">
         <f t="shared" si="14"/>
-        <v>1759.27734375</v>
+        <v>1198.5549926757812</v>
       </c>
       <c r="AE24" s="8">
-        <v>4.222546115215664E-4</v>
+        <v>3.2093251491005503E-4</v>
       </c>
       <c r="AF24" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2754364013672</v>
+        <v>1198.5530853271484</v>
       </c>
       <c r="AG24" s="8">
-        <v>1.4740981623617699E-4</v>
+        <v>-6.1019462509648292E-4</v>
       </c>
       <c r="AH24" s="8">
         <f t="shared" si="10"/>
-        <v>-1.8785323167514503E-8</v>
+        <v>9.4050646125482422E-7</v>
       </c>
       <c r="AI24" s="8">
         <f t="shared" si="11"/>
-        <v>6.2244474689272409E-8</v>
+        <v>-1.9583129561681245E-7</v>
       </c>
       <c r="AJ24" s="8">
         <f t="shared" si="12"/>
@@ -8872,14 +8947,14 @@
         <v>22</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>1.2999999999999601</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>101</v>
       </c>
       <c r="G25">
         <f xml:space="preserve"> 0.0268 * $C$20</f>
-        <v>47.148554294912174</v>
+        <v>32.121256186583928</v>
       </c>
       <c r="H25" t="s">
         <v>14</v>
@@ -8889,7 +8964,7 @@
       </c>
       <c r="K25">
         <f xml:space="preserve"> K19 * $C$22 * K24 - $C$23 * SIN(K17)</f>
-        <v>4.6694761655656691</v>
+        <v>2.4711032395395378</v>
       </c>
       <c r="L25" t="s">
         <v>19</v>
@@ -8899,35 +8974,35 @@
       </c>
       <c r="Q25" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412288665771484</v>
+        <v>0.43081998825073242</v>
       </c>
       <c r="R25" s="8">
         <f t="shared" si="0"/>
-        <v>1.136156879688599E-7</v>
+        <v>3.0482892765526515E-8</v>
       </c>
       <c r="S25" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412336349487305</v>
+        <v>0.43082046508789062</v>
       </c>
       <c r="T25" s="8">
         <f t="shared" si="1"/>
-        <v>-4.0042620375047022E-7</v>
+        <v>-4.6678869902727627E-7</v>
       </c>
       <c r="U25" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412312507629395</v>
+        <v>0.43082022666931152</v>
       </c>
       <c r="V25" s="8">
         <f t="shared" si="2"/>
-        <v>-1.4340527065836994E-7</v>
+        <v>-2.1815290873750115E-7</v>
       </c>
       <c r="W25" s="8">
         <f t="shared" si="4"/>
-        <v>-1.629308848421126E-14</v>
+        <v>-6.6499317235329396E-15</v>
       </c>
       <c r="X25" s="8">
         <f t="shared" si="5"/>
-        <v>5.7423228127539771E-14</v>
+        <v>1.0183131245859429E-13</v>
       </c>
       <c r="Y25" s="8">
         <f t="shared" si="6"/>
@@ -8938,32 +9013,32 @@
       </c>
       <c r="AB25" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2735290527344</v>
+        <v>1198.5530853271484</v>
       </c>
       <c r="AC25" s="8">
-        <v>-1.2743603952003468E-4</v>
+        <v>-6.1019462509648292E-4</v>
       </c>
       <c r="AD25" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2754364013672</v>
+        <v>1198.5549926757812</v>
       </c>
       <c r="AE25" s="8">
-        <v>1.4740981623617699E-4</v>
+        <v>3.2093251491005503E-4</v>
       </c>
       <c r="AF25" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744827270508</v>
+        <v>1198.5540390014648</v>
       </c>
       <c r="AG25" s="8">
-        <v>1.0811382026076899E-5</v>
+        <v>-1.4442584836160677E-4</v>
       </c>
       <c r="AH25" s="8">
         <f t="shared" si="10"/>
-        <v>-1.3777597071413283E-9</v>
+        <v>8.8127876395252129E-8</v>
       </c>
       <c r="AI25" s="8">
         <f t="shared" si="11"/>
-        <v>1.5937038377231026E-9</v>
+        <v>-4.6350950732708712E-8</v>
       </c>
       <c r="AJ25" s="8">
         <f t="shared" si="12"/>
@@ -8976,7 +9051,7 @@
       </c>
       <c r="G26">
         <f xml:space="preserve"> 11.5 * ($C$20*2.20462/1000)^0.4 * 0.453592</f>
-        <v>8.9707790153142888</v>
+        <v>7.6941352232120019</v>
       </c>
       <c r="H26" t="s">
         <v>14</v>
@@ -8986,42 +9061,42 @@
       </c>
       <c r="K26">
         <f xml:space="preserve"> 1/$C$9 - K23 * SQRT( (2*$C$33*PI()*$C$22^2) / K18^3 )</f>
-        <v>1.2247552694509789</v>
+        <v>1.1972131715570866</v>
       </c>
       <c r="P26" s="8">
         <v>22</v>
       </c>
       <c r="Q26" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412288665771484</v>
+        <v>0.43081998825073242</v>
       </c>
       <c r="R26" s="8">
         <f t="shared" si="0"/>
-        <v>1.136156879688599E-7</v>
+        <v>3.0482892765526515E-8</v>
       </c>
       <c r="S26" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412312507629395</v>
+        <v>0.43082022666931152</v>
       </c>
       <c r="T26" s="8">
         <f t="shared" si="1"/>
-        <v>-1.4340527065836994E-7</v>
+        <v>-2.1815290873750115E-7</v>
       </c>
       <c r="U26" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412300586700439</v>
+        <v>0.43082010746002197</v>
       </c>
       <c r="V26" s="8">
         <f t="shared" si="2"/>
-        <v>-1.4894794508890641E-8</v>
+        <v>-9.3835009373766098E-8</v>
       </c>
       <c r="W26" s="8">
         <f t="shared" si="4"/>
-        <v>-1.692282325282407E-15</v>
+        <v>-2.8603625283926874E-15</v>
       </c>
       <c r="X26" s="8">
         <f t="shared" si="5"/>
-        <v>2.1359920379482649E-15</v>
+        <v>2.047038023629776E-14</v>
       </c>
       <c r="Y26" s="8">
         <f t="shared" si="6"/>
@@ -9032,32 +9107,32 @@
       </c>
       <c r="AB26" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2735290527344</v>
+        <v>1198.5540390014648</v>
       </c>
       <c r="AC26" s="8">
-        <v>-1.2743603952003468E-4</v>
+        <v>-1.4442584836160677E-4</v>
       </c>
       <c r="AD26" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744827270508</v>
+        <v>1198.5549926757812</v>
       </c>
       <c r="AE26" s="8">
-        <v>1.0811382026076899E-5</v>
+        <v>3.2093251491005503E-4</v>
       </c>
       <c r="AF26" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2740058898926</v>
+        <v>1198.554515838623</v>
       </c>
       <c r="AG26" s="8">
-        <v>-5.7487935009703506E-5</v>
+        <v>8.8253343619726365E-5</v>
       </c>
       <c r="AH26" s="8">
         <f t="shared" si="10"/>
-        <v>7.3260347578217612E-9</v>
+        <v>-1.2746064023027376E-8</v>
       </c>
       <c r="AI26" s="8">
         <f t="shared" si="11"/>
-        <v>-6.2152402728018538E-10</v>
+        <v>2.8323367517100041E-8</v>
       </c>
       <c r="AJ26" s="8">
         <f t="shared" si="12"/>
@@ -9065,17 +9140,17 @@
       </c>
     </row>
     <row r="27" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
       <c r="F27" s="15" t="s">
         <v>103</v>
       </c>
       <c r="G27">
         <f xml:space="preserve"> 8 * ($C$20/1000)</f>
-        <v>14.074195311914082</v>
+        <v>9.5884346825623652</v>
       </c>
       <c r="H27" t="s">
         <v>14</v>
@@ -9091,35 +9166,35 @@
       </c>
       <c r="Q27" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412288665771484</v>
+        <v>0.43081998825073242</v>
       </c>
       <c r="R27" s="8">
         <f t="shared" si="0"/>
-        <v>1.136156879688599E-7</v>
+        <v>3.0482892765526515E-8</v>
       </c>
       <c r="S27" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412300586700439</v>
+        <v>0.43082010746002197</v>
       </c>
       <c r="T27" s="8">
         <f t="shared" si="1"/>
-        <v>-1.4894794508890641E-8</v>
+        <v>-9.3835009373766098E-8</v>
       </c>
       <c r="U27" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412294626235962</v>
+        <v>0.4308200478553772</v>
       </c>
       <c r="V27" s="8">
         <f t="shared" si="2"/>
-        <v>4.9360445897317362E-8</v>
+        <v>-3.1676058664942275E-8</v>
       </c>
       <c r="W27" s="8">
         <f t="shared" si="4"/>
-        <v>5.6081210190734E-15</v>
+        <v>-9.6557789951796239E-16</v>
       </c>
       <c r="X27" s="8">
         <f t="shared" si="5"/>
-        <v>-7.3521369850775619E-16</v>
+        <v>2.9723232617488233E-15</v>
       </c>
       <c r="Y27" s="8">
         <f t="shared" si="6"/>
@@ -9130,32 +9205,32 @@
       </c>
       <c r="AB27" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2740058898926</v>
+        <v>1198.5540390014648</v>
       </c>
       <c r="AC27" s="8">
-        <v>-5.7487935009703506E-5</v>
+        <v>-1.4442584836160677E-4</v>
       </c>
       <c r="AD27" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744827270508</v>
+        <v>1198.554515838623</v>
       </c>
       <c r="AE27" s="8">
-        <v>1.0811382026076899E-5</v>
+        <v>8.8253343619726365E-5</v>
       </c>
       <c r="AF27" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2742443084717</v>
+        <v>1198.5542774200439</v>
       </c>
       <c r="AG27" s="8">
-        <v>-2.4162629188140272E-5</v>
+        <v>-2.8291414537306991E-5</v>
       </c>
       <c r="AH27" s="8">
         <f t="shared" si="10"/>
-        <v>1.3890596564313729E-9</v>
+        <v>4.086011545900457E-9</v>
       </c>
       <c r="AI27" s="8">
         <f t="shared" si="11"/>
-        <v>-2.6123141490742079E-10</v>
+        <v>-2.4968119286490758E-9</v>
       </c>
       <c r="AJ27" s="8">
         <f t="shared" si="12"/>
@@ -9177,7 +9252,7 @@
       </c>
       <c r="G28">
         <f xml:space="preserve"> 13 * ($C$20*2.20462/1000)^1.3 * 0.453592</f>
-        <v>34.346008020428975</v>
+        <v>20.854397619186699</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
@@ -9187,42 +9262,42 @@
       </c>
       <c r="K28">
         <f xml:space="preserve"> 1/$C$38 * LN( EXP($C$38 * K26) + EXP($C$38 * K27) )</f>
-        <v>1.2281189006558431</v>
+        <v>1.2044530196453378</v>
       </c>
       <c r="P28" s="8">
         <v>24</v>
       </c>
       <c r="Q28" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412294626235962</v>
+        <v>0.43081998825073242</v>
       </c>
       <c r="R28" s="8">
         <f t="shared" si="0"/>
-        <v>4.9360445897317362E-8</v>
+        <v>3.0482892765526515E-8</v>
       </c>
       <c r="S28" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412300586700439</v>
+        <v>0.4308200478553772</v>
       </c>
       <c r="T28" s="8">
         <f t="shared" si="1"/>
-        <v>-1.4894794508890641E-8</v>
+        <v>-3.1676058664942275E-8</v>
       </c>
       <c r="U28" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412297606468201</v>
+        <v>0.43082001805305481</v>
       </c>
       <c r="V28" s="8">
         <f t="shared" si="2"/>
-        <v>1.7232825499924331E-8</v>
+        <v>-5.9658300521903129E-10</v>
       </c>
       <c r="W28" s="8">
         <f t="shared" si="4"/>
-        <v>8.5061995074692596E-16</v>
+        <v>-1.8185575773827276E-17</v>
       </c>
       <c r="X28" s="8">
         <f t="shared" si="5"/>
-        <v>-2.5667939462894357E-16</v>
+        <v>1.8897398271825599E-17</v>
       </c>
       <c r="Y28" s="8">
         <f t="shared" si="6"/>
@@ -9233,32 +9308,32 @@
       </c>
       <c r="AB28" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2742443084717</v>
+        <v>1198.5542774200439</v>
       </c>
       <c r="AC28" s="8">
-        <v>-2.4162629188140272E-5</v>
+        <v>-2.8291414537306991E-5</v>
       </c>
       <c r="AD28" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744827270508</v>
+        <v>1198.554515838623</v>
       </c>
       <c r="AE28" s="8">
-        <v>1.0811382026076899E-5</v>
+        <v>8.8253343619726365E-5</v>
       </c>
       <c r="AF28" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2743635177612</v>
+        <v>1198.5543966293335</v>
       </c>
       <c r="AG28" s="8">
-        <v>-7.49998253013473E-6</v>
+        <v>2.9980965337017551E-5</v>
       </c>
       <c r="AH28" s="8">
         <f t="shared" si="10"/>
-        <v>1.8121929679317556E-10</v>
+        <v>-8.4820391857819535E-10</v>
       </c>
       <c r="AI28" s="8">
         <f t="shared" si="11"/>
-        <v>-8.1085176322189364E-11</v>
+        <v>2.6459204359389152E-9</v>
       </c>
       <c r="AJ28" s="8">
         <f t="shared" si="12"/>
@@ -9270,7 +9345,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="1">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
@@ -9280,7 +9355,7 @@
       </c>
       <c r="G29" s="3">
         <f>$C$20 - $C$28 - SUM(G17:G28)</f>
-        <v>1.546140993013978E-10</v>
+        <v>-1.0618350643198937E-10</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>14</v>
@@ -9290,35 +9365,35 @@
       </c>
       <c r="Q29" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412297606468201</v>
+        <v>0.43081998825073242</v>
       </c>
       <c r="R29" s="8">
         <f t="shared" si="0"/>
-        <v>1.7232825499924331E-8</v>
+        <v>3.0482892765526515E-8</v>
       </c>
       <c r="S29" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412300586700439</v>
+        <v>0.43082001805305481</v>
       </c>
       <c r="T29" s="8">
         <f t="shared" si="1"/>
-        <v>-1.4894794508890641E-8</v>
+        <v>-5.9658300521903129E-10</v>
       </c>
       <c r="U29" s="8">
         <f t="shared" si="3"/>
-        <v>0.3441229909658432</v>
+        <v>0.43082000315189362</v>
       </c>
       <c r="V29" s="8">
         <f t="shared" si="2"/>
-        <v>1.169015440005694E-9</v>
+        <v>1.4943154880153742E-8</v>
       </c>
       <c r="W29" s="8">
         <f t="shared" si="4"/>
-        <v>2.0145439084335386E-17</v>
+        <v>4.5551058779038076E-16</v>
       </c>
       <c r="X29" s="8">
         <f t="shared" si="5"/>
-        <v>-1.7412244756605188E-17</v>
+        <v>-8.9148322458555526E-18</v>
       </c>
       <c r="Y29" s="8">
         <f t="shared" si="6"/>
@@ -9329,32 +9404,32 @@
       </c>
       <c r="AB29" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2743635177612</v>
+        <v>1198.5542774200439</v>
       </c>
       <c r="AC29" s="8">
-        <v>-7.49998253013473E-6</v>
+        <v>-2.8291414537306991E-5</v>
       </c>
       <c r="AD29" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744827270508</v>
+        <v>1198.5543966293335</v>
       </c>
       <c r="AE29" s="8">
-        <v>1.0811382026076899E-5</v>
+        <v>2.9980965337017551E-5</v>
       </c>
       <c r="AF29" s="8">
         <f t="shared" si="9"/>
-        <v>1759.274423122406</v>
+        <v>1198.5543370246887</v>
       </c>
       <c r="AG29" s="8">
-        <v>1.655700316405273E-6</v>
+        <v>8.4477562722895527E-7</v>
       </c>
       <c r="AH29" s="8">
         <f t="shared" si="10"/>
-        <v>-1.2417723448178093E-11</v>
+        <v>-2.3899897460947897E-11</v>
       </c>
       <c r="AI29" s="8">
         <f t="shared" si="11"/>
-        <v>1.7900408641353803E-11</v>
+        <v>2.5327188797508568E-11</v>
       </c>
       <c r="AJ29" s="8">
         <f t="shared" si="12"/>
@@ -9383,35 +9458,35 @@
       </c>
       <c r="Q30" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441229909658432</v>
+        <v>0.43082000315189362</v>
       </c>
       <c r="R30" s="8">
         <f t="shared" si="0"/>
-        <v>1.169015440005694E-9</v>
+        <v>1.4943154880153742E-8</v>
       </c>
       <c r="S30" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412300586700439</v>
+        <v>0.43082001805305481</v>
       </c>
       <c r="T30" s="8">
         <f t="shared" si="1"/>
-        <v>-1.4894794508890641E-8</v>
+        <v>-5.9658300521903129E-10</v>
       </c>
       <c r="U30" s="8">
         <f t="shared" si="3"/>
-        <v>0.3441229984164238</v>
+        <v>0.43082001060247421</v>
       </c>
       <c r="V30" s="8">
         <f t="shared" si="2"/>
-        <v>-6.8628895899536246E-9</v>
+        <v>7.1732859097117796E-9</v>
       </c>
       <c r="W30" s="8">
         <f t="shared" si="4"/>
-        <v>-8.0228238937101335E-18</v>
+        <v>1.0719152234844765E-16</v>
       </c>
       <c r="X30" s="8">
         <f t="shared" si="5"/>
-        <v>1.0222133017956399E-16</v>
+        <v>-4.2794604653111862E-18</v>
       </c>
       <c r="Y30" s="8">
         <f t="shared" si="6"/>
@@ -9422,32 +9497,32 @@
       </c>
       <c r="AB30" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2743635177612</v>
+        <v>1198.5542774200439</v>
       </c>
       <c r="AC30" s="8">
-        <v>-7.49998253013473E-6</v>
+        <v>-2.8291414537306991E-5</v>
       </c>
       <c r="AD30" s="8">
         <f t="shared" si="14"/>
-        <v>1759.274423122406</v>
+        <v>1198.5543370246887</v>
       </c>
       <c r="AE30" s="8">
-        <v>1.655700316405273E-6</v>
+        <v>8.4477562722895527E-7</v>
       </c>
       <c r="AF30" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2743933200836</v>
+        <v>1198.5543072223663</v>
       </c>
       <c r="AG30" s="8">
-        <v>-2.0977797703380929E-6</v>
+        <v>-1.3518154560188123E-5</v>
       </c>
       <c r="AH30" s="8">
         <f t="shared" si="10"/>
-        <v>1.5733311629605743E-11</v>
+        <v>3.8244771444166902E-10</v>
       </c>
       <c r="AI30" s="8">
         <f t="shared" si="11"/>
-        <v>-3.4732946294973615E-12</v>
+        <v>-1.1419807497560883E-11</v>
       </c>
       <c r="AJ30" s="8">
         <f t="shared" si="12"/>
@@ -9460,35 +9535,35 @@
       </c>
       <c r="Q31" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441229909658432</v>
+        <v>0.43082001060247421</v>
       </c>
       <c r="R31" s="8">
         <f t="shared" si="0"/>
-        <v>1.169015440005694E-9</v>
+        <v>7.1732859097117796E-9</v>
       </c>
       <c r="S31" s="8">
         <f t="shared" si="8"/>
-        <v>0.3441229984164238</v>
+        <v>0.43082001805305481</v>
       </c>
       <c r="T31" s="8">
         <f t="shared" si="1"/>
-        <v>-6.8628895899536246E-9</v>
+        <v>-5.9658300521903129E-10</v>
       </c>
       <c r="U31" s="8">
         <f t="shared" si="3"/>
-        <v>0.3441229946911335</v>
+        <v>0.43082001432776451</v>
       </c>
       <c r="V31" s="8">
         <f t="shared" si="2"/>
-        <v>-2.8469370749739653E-9</v>
+        <v>3.2883514800019498E-9</v>
       </c>
       <c r="W31" s="8">
         <f t="shared" si="4"/>
-        <v>-3.3281133973692136E-18</v>
+        <v>2.3588285337677863E-17</v>
       </c>
       <c r="X31" s="8">
         <f t="shared" si="5"/>
-        <v>1.9538214815091848E-17</v>
+        <v>-1.9617746081560125E-18</v>
       </c>
       <c r="Y31" s="8">
         <f t="shared" si="6"/>
@@ -9499,32 +9574,32 @@
       </c>
       <c r="AB31" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2743933200836</v>
+        <v>1198.5543072223663</v>
       </c>
       <c r="AC31" s="8">
-        <v>-2.0977797703380929E-6</v>
+        <v>-1.3518154560188123E-5</v>
       </c>
       <c r="AD31" s="8">
         <f t="shared" si="14"/>
-        <v>1759.274423122406</v>
+        <v>1198.5543370246887</v>
       </c>
       <c r="AE31" s="8">
-        <v>1.655700316405273E-6</v>
+        <v>8.4477562722895527E-7</v>
       </c>
       <c r="AF31" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744082212448</v>
+        <v>1198.5543221235275</v>
       </c>
       <c r="AG31" s="8">
-        <v>-1.0454011771798832E-6</v>
+        <v>-6.5418543044870603E-6</v>
       </c>
       <c r="AH31" s="8">
         <f t="shared" si="10"/>
-        <v>2.1930214413755874E-12</v>
+        <v>8.8433797598288053E-11</v>
       </c>
       <c r="AI31" s="8">
         <f t="shared" si="11"/>
-        <v>-1.7308710598271776E-12</v>
+        <v>-5.5263990733134973E-12</v>
       </c>
       <c r="AJ31" s="8">
         <f t="shared" si="12"/>
@@ -9532,45 +9607,45 @@
       </c>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
       <c r="P32" s="8">
         <v>28</v>
       </c>
       <c r="Q32" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441229909658432</v>
+        <v>0.43082001432776451</v>
       </c>
       <c r="R32" s="8">
         <f t="shared" si="0"/>
-        <v>1.169015440005694E-9</v>
+        <v>3.2883514800019498E-9</v>
       </c>
       <c r="S32" s="8">
         <f t="shared" si="8"/>
-        <v>0.3441229946911335</v>
+        <v>0.43082001805305481</v>
       </c>
       <c r="T32" s="8">
         <f t="shared" si="1"/>
-        <v>-2.8469370749739653E-9</v>
+        <v>-5.9658300521903129E-10</v>
       </c>
       <c r="U32" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412299282848835</v>
+        <v>0.43082001619040966</v>
       </c>
       <c r="V32" s="8">
         <f t="shared" si="2"/>
-        <v>-8.3896084523971126E-10</v>
+        <v>1.3458842373914592E-9</v>
       </c>
       <c r="W32" s="8">
         <f t="shared" si="4"/>
-        <v>-9.8075818164545002E-19</v>
+        <v>4.4257404239375005E-18</v>
       </c>
       <c r="X32" s="8">
         <f t="shared" si="5"/>
-        <v>2.3884687347644292E-18</v>
+        <v>-8.0293166301992088E-19</v>
       </c>
       <c r="Y32" s="8">
         <f t="shared" si="6"/>
@@ -9581,32 +9656,32 @@
       </c>
       <c r="AB32" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744082212448</v>
+        <v>1198.5543221235275</v>
       </c>
       <c r="AC32" s="8">
-        <v>-1.0454011771798832E-6</v>
+        <v>-6.5418543044870603E-6</v>
       </c>
       <c r="AD32" s="8">
         <f t="shared" si="14"/>
-        <v>1759.274423122406</v>
+        <v>1198.5543370246887</v>
       </c>
       <c r="AE32" s="8">
-        <v>1.655700316405273E-6</v>
+        <v>8.4477562722895527E-7</v>
       </c>
       <c r="AF32" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744156718254</v>
+        <v>1198.5543295741081</v>
       </c>
       <c r="AG32" s="8">
-        <v>3.0514979698637035E-7</v>
+        <v>-2.848539566002728E-6</v>
       </c>
       <c r="AH32" s="8">
         <f t="shared" si="10"/>
-        <v>-3.1900395698575395E-13</v>
+        <v>1.8634730821356648E-11</v>
       </c>
       <c r="AI32" s="8">
         <f t="shared" si="11"/>
-        <v>5.0523661542133822E-13</v>
+        <v>-2.4063767985564505E-12</v>
       </c>
       <c r="AJ32" s="8">
         <f t="shared" si="12"/>
@@ -9633,35 +9708,35 @@
       </c>
       <c r="Q33" s="8">
         <f t="shared" si="7"/>
-        <v>0.3441229909658432</v>
+        <v>0.43082001619040966</v>
       </c>
       <c r="R33" s="8">
         <f t="shared" si="0"/>
-        <v>1.169015440005694E-9</v>
+        <v>1.3458842373914592E-9</v>
       </c>
       <c r="S33" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412299282848835</v>
+        <v>0.43082001805305481</v>
       </c>
       <c r="T33" s="8">
         <f t="shared" si="1"/>
-        <v>-8.3896084523971126E-10</v>
+        <v>-5.9658300521903129E-10</v>
       </c>
       <c r="U33" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412299189716578</v>
+        <v>0.43082001712173223</v>
       </c>
       <c r="V33" s="8">
         <f t="shared" si="2"/>
-        <v>1.6502732513856699E-10</v>
+        <v>3.7465058833063836E-10</v>
       </c>
       <c r="W33" s="8">
         <f t="shared" si="4"/>
-        <v>1.9291949110982462E-19</v>
+        <v>5.0423632136364274E-19</v>
       </c>
       <c r="X33" s="8">
         <f t="shared" si="5"/>
-        <v>-1.3845146418590082E-19</v>
+        <v>-2.2351017389337037E-19</v>
       </c>
       <c r="Y33" s="8">
         <f t="shared" si="6"/>
@@ -9672,32 +9747,32 @@
       </c>
       <c r="AB33" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744082212448</v>
+        <v>1198.5543295741081</v>
       </c>
       <c r="AC33" s="8">
-        <v>-1.0454011771798832E-6</v>
+        <v>-2.848539566002728E-6</v>
       </c>
       <c r="AD33" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744156718254</v>
+        <v>1198.5543370246887</v>
       </c>
       <c r="AE33" s="8">
-        <v>3.0514979698637035E-7</v>
+        <v>8.4477562722895527E-7</v>
       </c>
       <c r="AF33" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744119465351</v>
+        <v>1198.5543332993984</v>
       </c>
       <c r="AG33" s="8">
-        <v>-3.7012591747043189E-7</v>
+        <v>-1.0018820830737241E-6</v>
       </c>
       <c r="AH33" s="8">
         <f t="shared" si="10"/>
-        <v>3.869300698283738E-13</v>
+        <v>2.853900754104735E-12</v>
       </c>
       <c r="AI33" s="8">
         <f t="shared" si="11"/>
-        <v>-1.1294384857549636E-13</v>
+        <v>-8.4636556513805752E-13</v>
       </c>
       <c r="AJ33" s="8">
         <f t="shared" si="12"/>
@@ -9719,7 +9794,7 @@
       </c>
       <c r="G34">
         <f>ROUND($C$28/$C$20 * 100, 2)</f>
-        <v>22.74</v>
+        <v>33.369999999999997</v>
       </c>
       <c r="H34" t="s">
         <v>95</v>
@@ -9729,35 +9804,35 @@
       </c>
       <c r="Q34" s="8">
         <f t="shared" si="7"/>
-        <v>0.34412299189716578</v>
+        <v>0.43082001712173223</v>
       </c>
       <c r="R34" s="8">
         <f t="shared" si="0"/>
-        <v>1.6502732513856699E-10</v>
+        <v>3.7465058833063836E-10</v>
       </c>
       <c r="S34" s="8">
         <f t="shared" si="8"/>
-        <v>0.34412299282848835</v>
+        <v>0.43082001805305481</v>
       </c>
       <c r="T34" s="8">
         <f t="shared" si="1"/>
-        <v>-8.3896084523971126E-10</v>
+        <v>-5.9658300521903129E-10</v>
       </c>
       <c r="U34" s="8">
         <f t="shared" si="3"/>
-        <v>0.34412299236282706</v>
+        <v>0.43082001758739352</v>
       </c>
       <c r="V34" s="8">
         <f t="shared" si="2"/>
-        <v>-3.3696678780614775E-10</v>
+        <v>-1.1096623619977208E-10</v>
       </c>
       <c r="W34" s="8">
         <f t="shared" si="4"/>
-        <v>-5.5608727652183656E-20</v>
+        <v>-4.1573565677081191E-20</v>
       </c>
       <c r="X34" s="8">
         <f t="shared" si="5"/>
-        <v>2.8270194111555615E-19</v>
+        <v>6.6200570669904888E-20</v>
       </c>
       <c r="Y34" s="8">
         <f t="shared" si="6"/>
@@ -9768,32 +9843,32 @@
       </c>
       <c r="AB34" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744119465351</v>
+        <v>1198.5543332993984</v>
       </c>
       <c r="AC34" s="8">
-        <v>-3.7012591747043189E-7</v>
+        <v>-1.0018820830737241E-6</v>
       </c>
       <c r="AD34" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744156718254</v>
+        <v>1198.5543370246887</v>
       </c>
       <c r="AE34" s="8">
-        <v>3.0514979698637035E-7</v>
+        <v>8.4477562722895527E-7</v>
       </c>
       <c r="AF34" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744138091803</v>
+        <v>1198.5543351620436</v>
       </c>
       <c r="AG34" s="8">
-        <v>-3.248806024203077E-8</v>
+        <v>-7.8553057392127812E-8</v>
       </c>
       <c r="AH34" s="8">
         <f t="shared" si="10"/>
-        <v>1.20246731039163E-14</v>
+        <v>7.870090077183481E-14</v>
       </c>
       <c r="AI34" s="8">
         <f t="shared" si="11"/>
-        <v>-9.9137249873366592E-15</v>
+        <v>-6.6359708329186894E-14</v>
       </c>
       <c r="AJ34" s="8">
         <f t="shared" si="12"/>
@@ -9815,7 +9890,7 @@
       </c>
       <c r="G35">
         <f>ROUND(G17/$C$20 * 100, 2)</f>
-        <v>35.69</v>
+        <v>17.57</v>
       </c>
       <c r="H35" t="s">
         <v>95</v>
@@ -9825,32 +9900,32 @@
       </c>
       <c r="AB35" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744138091803</v>
+        <v>1198.5543351620436</v>
       </c>
       <c r="AC35">
-        <v>-3.248806024203077E-8</v>
+        <v>-7.8553057392127812E-8</v>
       </c>
       <c r="AD35" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744156718254</v>
+        <v>1198.5543370246887</v>
       </c>
       <c r="AE35">
-        <v>3.0514979698637035E-7</v>
+        <v>8.4477562722895527E-7</v>
       </c>
       <c r="AF35" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744147405028</v>
+        <v>1198.5543360933661</v>
       </c>
       <c r="AG35">
-        <v>1.3633098205900751E-7</v>
+        <v>3.8311111438815715E-7</v>
       </c>
       <c r="AH35" s="8">
         <f t="shared" si="10"/>
-        <v>-4.429129157988252E-15</v>
+        <v>-3.0094549356094952E-14</v>
       </c>
       <c r="AI35" s="8">
         <f t="shared" si="11"/>
-        <v>4.160137149825864E-14</v>
+        <v>3.2364293195563949E-13</v>
       </c>
       <c r="AJ35" s="8">
         <f t="shared" si="12"/>
@@ -9863,7 +9938,7 @@
       </c>
       <c r="G36">
         <f>ROUND(SUM(G18:G19)/$C$20 * 100, 2)</f>
-        <v>13.12</v>
+        <v>11.01</v>
       </c>
       <c r="H36" t="s">
         <v>95</v>
@@ -9873,32 +9948,32 @@
       </c>
       <c r="AB36" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744138091803</v>
+        <v>1198.5543351620436</v>
       </c>
       <c r="AC36">
-        <v>-3.248806024203077E-8</v>
+        <v>-7.8553057392127812E-8</v>
       </c>
       <c r="AD36" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744147405028</v>
+        <v>1198.5543360933661</v>
       </c>
       <c r="AE36">
-        <v>1.3633098205900751E-7</v>
+        <v>3.8311111438815715E-7</v>
       </c>
       <c r="AF36" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744142748415</v>
+        <v>1198.5543356277049</v>
       </c>
       <c r="AG36">
-        <v>5.1921006161137484E-8</v>
+        <v>1.5227908534143353E-7</v>
       </c>
       <c r="AH36" s="8">
         <f t="shared" si="10"/>
-        <v>-1.6868127759898853E-15</v>
+        <v>-1.1961987730446357E-14</v>
       </c>
       <c r="AI36" s="8">
         <f t="shared" si="11"/>
-        <v>7.0784417594396528E-15</v>
+        <v>5.8339810083165885E-14</v>
       </c>
       <c r="AJ36" s="8">
         <f t="shared" si="12"/>
@@ -9906,17 +9981,17 @@
       </c>
     </row>
     <row r="37" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
       <c r="F37" s="17" t="s">
         <v>108</v>
       </c>
       <c r="G37">
         <f>ROUND(SUM(G20:G24)/$C$20 * 100, 2)</f>
-        <v>22.51</v>
+        <v>32.18</v>
       </c>
       <c r="H37" t="s">
         <v>95</v>
@@ -9926,32 +10001,32 @@
       </c>
       <c r="AB37" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744138091803</v>
+        <v>1198.5543351620436</v>
       </c>
       <c r="AC37">
-        <v>-3.248806024203077E-8</v>
+        <v>-7.8553057392127812E-8</v>
       </c>
       <c r="AD37" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744142748415</v>
+        <v>1198.5543356277049</v>
       </c>
       <c r="AE37">
-        <v>5.1921006161137484E-8</v>
+        <v>1.5227908534143353E-7</v>
       </c>
       <c r="AF37" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744140420109</v>
+        <v>1198.5543353948742</v>
       </c>
       <c r="AG37">
-        <v>9.7161318990401924E-9</v>
+        <v>3.6862957131233998E-8</v>
       </c>
       <c r="AH37" s="8">
         <f t="shared" si="10"/>
-        <v>-3.1565827845553459E-16</v>
+        <v>-2.8956979871733714E-15</v>
       </c>
       <c r="AI37" s="8">
         <f t="shared" si="11"/>
-        <v>5.0447134419249027E-16</v>
+        <v>5.6134573949247876E-15</v>
       </c>
       <c r="AJ37" s="8">
         <f t="shared" si="12"/>
@@ -9970,7 +10045,7 @@
       </c>
       <c r="G38">
         <f>ROUND(SUM(G25:G28)/$C$20*100, 2)</f>
-        <v>5.94</v>
+        <v>5.86</v>
       </c>
       <c r="H38" t="s">
         <v>95</v>
@@ -9980,32 +10055,32 @@
       </c>
       <c r="AB38" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744138091803</v>
+        <v>1198.5543351620436</v>
       </c>
       <c r="AC38">
-        <v>-3.248806024203077E-8</v>
+        <v>-7.8553057392127812E-8</v>
       </c>
       <c r="AD38" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744140420109</v>
+        <v>1198.5543353948742</v>
       </c>
       <c r="AE38">
-        <v>9.7161318990401924E-9</v>
+        <v>3.6862957131233998E-8</v>
       </c>
       <c r="AF38" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744139255956</v>
+        <v>1198.5543352784589</v>
       </c>
       <c r="AG38">
-        <v>-1.1385736797819845E-8</v>
+        <v>-2.0844936443609186E-8</v>
       </c>
       <c r="AH38" s="8">
         <f t="shared" si="10"/>
-        <v>3.6990050298747765E-16</v>
+        <v>1.637433488790089E-15</v>
       </c>
       <c r="AI38" s="8">
         <f t="shared" si="11"/>
-        <v>-1.1062532049537313E-16</v>
+        <v>-7.6840599852406267E-16</v>
       </c>
       <c r="AJ38" s="8">
         <f t="shared" si="12"/>
@@ -10018,7 +10093,7 @@
       </c>
       <c r="G39" s="3">
         <f>SUM(G34:G38)</f>
-        <v>100</v>
+        <v>99.99</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>95</v>
@@ -10028,32 +10103,32 @@
       </c>
       <c r="AB39" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744139255956</v>
+        <v>1198.5543352784589</v>
       </c>
       <c r="AC39">
-        <v>-1.1385736797819845E-8</v>
+        <v>-2.0844936443609186E-8</v>
       </c>
       <c r="AD39" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744140420109</v>
+        <v>1198.5543353948742</v>
       </c>
       <c r="AE39">
-        <v>9.7161318990401924E-9</v>
+        <v>3.6862957131233998E-8</v>
       </c>
       <c r="AF39" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744139838032</v>
+        <v>1198.5543353366666</v>
       </c>
       <c r="AG39">
-        <v>-8.3491613622754812E-10</v>
+        <v>8.0087829701369628E-9</v>
       </c>
       <c r="AH39" s="8">
         <f t="shared" si="10"/>
-        <v>9.5061353753395616E-18</v>
+        <v>-1.6694257200316459E-16</v>
       </c>
       <c r="AI39" s="8">
         <f t="shared" si="11"/>
-        <v>-8.1121553042238671E-18</v>
+        <v>2.9522742330151575E-16</v>
       </c>
       <c r="AJ39" s="8">
         <f t="shared" si="12"/>
@@ -10066,32 +10141,32 @@
       </c>
       <c r="AB40" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744139838032</v>
+        <v>1198.5543352784589</v>
       </c>
       <c r="AC40">
-        <v>-8.3491613622754812E-10</v>
+        <v>-2.0844936443609186E-8</v>
       </c>
       <c r="AD40" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744140420109</v>
+        <v>1198.5543353366666</v>
       </c>
       <c r="AE40">
-        <v>9.7161318990401924E-9</v>
+        <v>8.0087829701369628E-9</v>
       </c>
       <c r="AF40" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744140129071</v>
+        <v>1198.5543353075627</v>
       </c>
       <c r="AG40">
-        <v>4.4410626287572086E-9</v>
+        <v>-6.418190423573833E-9</v>
       </c>
       <c r="AH40" s="8">
         <f t="shared" si="10"/>
-        <v>-3.7079148507465265E-18</v>
+        <v>1.3378677146237767E-16</v>
       </c>
       <c r="AI40" s="8">
         <f t="shared" si="11"/>
-        <v>4.3149950272903206E-17</v>
+        <v>-5.1401894163414253E-17</v>
       </c>
       <c r="AJ40" s="8">
         <f t="shared" si="12"/>
@@ -10099,37 +10174,40 @@
       </c>
     </row>
     <row r="41" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="C41" s="1">
+        <v>1.2</v>
+      </c>
       <c r="AA41" s="8">
         <v>37</v>
       </c>
       <c r="AB41" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744139838032</v>
+        <v>1198.5543353075627</v>
       </c>
       <c r="AC41">
-        <v>-8.3491613622754812E-10</v>
+        <v>-6.418190423573833E-9</v>
       </c>
       <c r="AD41" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744140129071</v>
+        <v>1198.5543353366666</v>
       </c>
       <c r="AE41">
-        <v>4.4410626287572086E-9</v>
+        <v>8.0087829701369628E-9</v>
       </c>
       <c r="AF41" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744139983552</v>
+        <v>1198.5543353221146</v>
       </c>
       <c r="AG41">
-        <v>1.8030732462648302E-9</v>
+        <v>7.9535311670042574E-10</v>
       </c>
       <c r="AH41" s="8">
         <f t="shared" si="10"/>
-        <v>-1.5054149481066944E-18</v>
+        <v>-5.1047277569662737E-18</v>
       </c>
       <c r="AI41" s="8">
         <f t="shared" si="11"/>
-        <v>8.0075612108986807E-18</v>
+        <v>6.3698104962757261E-18</v>
       </c>
       <c r="AJ41" s="8">
         <f t="shared" si="12"/>
@@ -10137,37 +10215,40 @@
       </c>
     </row>
     <row r="42" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="C42" s="1">
+        <v>0.9</v>
+      </c>
       <c r="AA42" s="8">
         <v>38</v>
       </c>
       <c r="AB42" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744139838032</v>
+        <v>1198.5543353075627</v>
       </c>
       <c r="AC42">
-        <v>-8.3491613622754812E-10</v>
+        <v>-6.418190423573833E-9</v>
       </c>
       <c r="AD42" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744139983552</v>
+        <v>1198.5543353221146</v>
       </c>
       <c r="AE42">
-        <v>1.8030732462648302E-9</v>
+        <v>7.9535311670042574E-10</v>
       </c>
       <c r="AF42" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744139910792</v>
+        <v>1198.5543353148387</v>
       </c>
       <c r="AG42">
-        <v>4.8430592869408429E-10</v>
+        <v>-2.8113618100178428E-9</v>
       </c>
       <c r="AH42" s="8">
         <f t="shared" si="10"/>
-        <v>-4.0435483473735928E-19</v>
+        <v>1.8043855446257716E-17</v>
       </c>
       <c r="AI42" s="8">
         <f t="shared" si="11"/>
-        <v>8.7323906303574595E-19</v>
+        <v>-2.2360253777702415E-18</v>
       </c>
       <c r="AJ42" s="8">
         <f t="shared" si="12"/>
@@ -10175,37 +10256,40 @@
       </c>
     </row>
     <row r="43" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="C43" s="1">
+        <v>55</v>
+      </c>
       <c r="AA43" s="8">
         <v>39</v>
       </c>
       <c r="AB43" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744139838032</v>
+        <v>1198.5543353148387</v>
       </c>
       <c r="AC43">
-        <v>-8.3491613622754812E-10</v>
+        <v>-2.8113618100178428E-9</v>
       </c>
       <c r="AD43" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744139910792</v>
+        <v>1198.5543353221146</v>
       </c>
       <c r="AE43">
-        <v>4.8430592869408429E-10</v>
+        <v>7.9535311670042574E-10</v>
       </c>
       <c r="AF43" s="8">
         <f t="shared" si="9"/>
-        <v>1759.2744139874412</v>
+        <v>1198.5543353184767</v>
       </c>
       <c r="AG43">
-        <v>-1.7530510376673192E-10</v>
+        <v>-1.0079475032398477E-9</v>
       </c>
       <c r="AH43" s="8">
         <f t="shared" si="10"/>
-        <v>1.4636505989788921E-19</v>
+        <v>2.8337051171113438E-18</v>
       </c>
       <c r="AI43" s="8">
         <f t="shared" si="11"/>
-        <v>-8.4901301084559915E-20</v>
+        <v>-8.0167418817222536E-19</v>
       </c>
       <c r="AJ43" s="8">
         <f t="shared" si="12"/>
@@ -10213,41 +10297,99 @@
       </c>
     </row>
     <row r="44" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="C44" s="1">
+        <v>6.4</v>
+      </c>
       <c r="AA44" s="8">
         <v>40</v>
       </c>
       <c r="AB44" s="8">
         <f t="shared" si="13"/>
-        <v>1759.2744139874412</v>
+        <v>1198.5543353184767</v>
       </c>
       <c r="AC44">
-        <v>-1.7530510376673192E-10</v>
+        <v>-1.0079475032398477E-9</v>
       </c>
       <c r="AD44" s="8">
         <f t="shared" si="14"/>
-        <v>1759.2744139910792</v>
+        <v>1198.5543353221146</v>
       </c>
       <c r="AE44">
-        <v>4.8430592869408429E-10</v>
+        <v>7.9535311670042574E-10</v>
       </c>
       <c r="AF44" s="11">
         <f t="shared" si="9"/>
-        <v>1759.2744139892602</v>
+        <v>1198.5543353202956</v>
       </c>
       <c r="AG44">
-        <v>1.546140993013978E-10</v>
+        <v>-1.0618350643198937E-10</v>
       </c>
       <c r="AH44" s="8">
         <f t="shared" si="10"/>
-        <v>-2.7104640721831334E-20</v>
+        <v>1.07027400193376E-19</v>
       </c>
       <c r="AI44" s="8">
         <f t="shared" si="11"/>
-        <v>7.488052495136283E-20</v>
+        <v>-8.445338278286245E-20</v>
       </c>
       <c r="AJ44" s="8">
         <f t="shared" si="12"/>
         <v>3.637978807091713E-9</v>
+      </c>
+    </row>
+    <row r="45" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="T45" t="s">
+        <v>140</v>
+      </c>
+      <c r="U45">
+        <v>10</v>
+      </c>
+      <c r="V45">
+        <v>10</v>
+      </c>
+      <c r="W45">
+        <v>10</v>
+      </c>
+      <c r="X45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="T46" t="s">
+        <v>139</v>
+      </c>
+      <c r="U46">
+        <f>U47^2/U45</f>
+        <v>6.4</v>
+      </c>
+      <c r="V46">
+        <f>V47^2/V45</f>
+        <v>3.6</v>
+      </c>
+      <c r="W46">
+        <f>W47^2/W45</f>
+        <v>14.4</v>
+      </c>
+      <c r="X46">
+        <f>X47^2/X45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="T47" t="s">
+        <v>79</v>
+      </c>
+      <c r="U47">
+        <v>8</v>
+      </c>
+      <c r="V47">
+        <v>6</v>
+      </c>
+      <c r="W47">
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="27:27" x14ac:dyDescent="0.2">
@@ -10299,4 +10441,215 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04399F6A-8712-2C4A-BDE2-261DEBFAF47B}">
+  <dimension ref="B2:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3">
+        <v>3269</v>
+      </c>
+      <c r="D3">
+        <v>2864</v>
+      </c>
+      <c r="E3">
+        <v>3858</v>
+      </c>
+      <c r="F3">
+        <v>4399</v>
+      </c>
+      <c r="G3">
+        <v>3863</v>
+      </c>
+      <c r="H3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5">
+        <v>6.6</v>
+      </c>
+      <c r="D5">
+        <v>25.9</v>
+      </c>
+      <c r="E5">
+        <v>4.7</v>
+      </c>
+      <c r="F5">
+        <v>5.2</v>
+      </c>
+      <c r="G5">
+        <v>15.8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6">
+        <f>2.5 * (C3/1000) ^ (2/3)</f>
+        <v>5.5065969395516792</v>
+      </c>
+      <c r="D6">
+        <f>0.0327*D3^0.8903</f>
+        <v>39.110271131161461</v>
+      </c>
+      <c r="E6">
+        <f>1.6 * (E3/1000) ^ (2/3)</f>
+        <v>3.9357556858069622</v>
+      </c>
+      <c r="F6">
+        <f>1.6 * (F3/1000) ^ (2/3)</f>
+        <v>4.2955880345721758</v>
+      </c>
+      <c r="G6">
+        <f>1.6 * (G3/1000) ^ (2/3)</f>
+        <v>3.9391554663896855</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7">
+        <f>C5/((C3/1000)^(2/3))</f>
+        <v>2.9964059801593814</v>
+      </c>
+      <c r="E7">
+        <f>E5/((E3/1000)^(2/3))</f>
+        <v>1.9106877053162785</v>
+      </c>
+      <c r="F7">
+        <f>F5/((F3/1000)^(2/3))</f>
+        <v>1.9368710251165047</v>
+      </c>
+      <c r="G7">
+        <f>G5/((G3/1000)^(2/3))</f>
+        <v>6.4176192627323809</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+      <c r="H13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17">
+        <v>0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>